<commit_message>
final commit to merge branches. Codebase used for Ph.D. experiments.
</commit_message>
<xml_diff>
--- a/assesmentData/IMAP Typologies E consumption per type with end uses.xlsx
+++ b/assesmentData/IMAP Typologies E consumption per type with end uses.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\angel\Documents\GitHub\gr4sp\experiments\notebookGr4sp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\angel\Documents\GitHub\gr4sp\experiments\assesmentData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{879860D0-C04A-4FA9-8EC8-1554845A3F80}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FDADF31-4084-4EEE-B650-D85003A4A349}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="225" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ImapEnergyIntensity with totals" sheetId="1" r:id="rId1"/>
@@ -1033,26 +1033,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T289"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="S113" sqref="S113:S115"/>
+      <selection pane="bottomLeft" activeCell="Z12" sqref="Z12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="17" customWidth="1"/>
-    <col min="3" max="3" width="14.5546875" customWidth="1"/>
-    <col min="4" max="4" width="24.6640625" customWidth="1"/>
-    <col min="5" max="5" width="23.33203125" customWidth="1"/>
-    <col min="6" max="6" width="13.6640625" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" customWidth="1"/>
+    <col min="4" max="4" width="24.7109375" customWidth="1"/>
+    <col min="5" max="5" width="23.28515625" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" customWidth="1"/>
     <col min="7" max="10" width="12" bestFit="1" customWidth="1"/>
     <col min="15" max="17" width="12" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="12" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="45.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1114,7 +1114,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -1170,14 +1170,14 @@
         <v>57</v>
       </c>
       <c r="S2" s="4">
-        <f>PRODUCT(Q2,R2)</f>
+        <f t="shared" ref="S2:S65" si="0">PRODUCT(Q2,R2)</f>
         <v>4936.0718497500002</v>
       </c>
       <c r="T2">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -1233,14 +1233,14 @@
         <v>57</v>
       </c>
       <c r="S3" s="4">
-        <f>PRODUCT(Q3,R3)</f>
+        <f t="shared" si="0"/>
         <v>5446.2731742599999</v>
       </c>
       <c r="T3">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -1296,14 +1296,14 @@
         <v>57</v>
       </c>
       <c r="S4" s="4">
-        <f>PRODUCT(Q4,R4)</f>
+        <f t="shared" si="0"/>
         <v>5517.2215770000003</v>
       </c>
       <c r="T4">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -1359,14 +1359,14 @@
         <v>57</v>
       </c>
       <c r="S5" s="4">
-        <f>PRODUCT(Q5,R5)</f>
+        <f t="shared" si="0"/>
         <v>5624.4338556899993</v>
       </c>
       <c r="T5">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -1422,14 +1422,14 @@
         <v>117</v>
       </c>
       <c r="S6" s="4">
-        <f>PRODUCT(Q6,R6)</f>
+        <f t="shared" si="0"/>
         <v>5659.0114358700002</v>
       </c>
       <c r="T6">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -1485,14 +1485,14 @@
         <v>57</v>
       </c>
       <c r="S7" s="4">
-        <f>PRODUCT(Q7,R7)</f>
+        <f t="shared" si="0"/>
         <v>5882.2030421999998</v>
       </c>
       <c r="T7">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -1548,14 +1548,14 @@
         <v>139</v>
       </c>
       <c r="S8" s="4">
-        <f>PRODUCT(Q8,R8)</f>
+        <f t="shared" si="0"/>
         <v>5940.2142810600008</v>
       </c>
       <c r="T8">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -1611,14 +1611,14 @@
         <v>139</v>
       </c>
       <c r="S9" s="4">
-        <f>PRODUCT(Q9,R9)</f>
+        <f t="shared" si="0"/>
         <v>5980.9886939600001</v>
       </c>
       <c r="T9">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>24</v>
       </c>
@@ -1674,14 +1674,14 @@
         <v>57</v>
       </c>
       <c r="S10" s="4">
-        <f>PRODUCT(Q10,R10)</f>
+        <f t="shared" si="0"/>
         <v>6131.3889219000002</v>
       </c>
       <c r="T10">
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>24</v>
       </c>
@@ -1737,14 +1737,14 @@
         <v>152</v>
       </c>
       <c r="S11" s="4">
-        <f>PRODUCT(Q11,R11)</f>
+        <f t="shared" si="0"/>
         <v>6161.8771438399999</v>
       </c>
       <c r="T11">
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -1800,14 +1800,14 @@
         <v>117</v>
       </c>
       <c r="S12" s="4">
-        <f>PRODUCT(Q12,R12)</f>
+        <f t="shared" si="0"/>
         <v>6198.4902330000004</v>
       </c>
       <c r="T12">
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -1863,14 +1863,14 @@
         <v>57</v>
       </c>
       <c r="S13" s="4">
-        <f>PRODUCT(Q13,R13)</f>
+        <f t="shared" si="0"/>
         <v>6207.3871130999996</v>
       </c>
       <c r="T13">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>22</v>
       </c>
@@ -1926,14 +1926,14 @@
         <v>117</v>
       </c>
       <c r="S14" s="4">
-        <f>PRODUCT(Q14,R14)</f>
+        <f t="shared" si="0"/>
         <v>6342.2980065900001</v>
       </c>
       <c r="T14">
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>24</v>
       </c>
@@ -1989,14 +1989,14 @@
         <v>57</v>
       </c>
       <c r="S15" s="4">
-        <f>PRODUCT(Q15,R15)</f>
+        <f t="shared" si="0"/>
         <v>6367.9825610999997</v>
       </c>
       <c r="T15">
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -2052,14 +2052,14 @@
         <v>139</v>
       </c>
       <c r="S16" s="4">
-        <f>PRODUCT(Q16,R16)</f>
+        <f t="shared" si="0"/>
         <v>6506.0371149899993</v>
       </c>
       <c r="T16">
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>23</v>
       </c>
@@ -2115,14 +2115,14 @@
         <v>57</v>
       </c>
       <c r="S17" s="4">
-        <f>PRODUCT(Q17,R17)</f>
+        <f t="shared" si="0"/>
         <v>6582.1030154999999</v>
       </c>
       <c r="T17">
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>23</v>
       </c>
@@ -2178,14 +2178,14 @@
         <v>139</v>
       </c>
       <c r="S18" s="4">
-        <f>PRODUCT(Q18,R18)</f>
+        <f t="shared" si="0"/>
         <v>6649.35652192</v>
       </c>
       <c r="T18">
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -2241,14 +2241,14 @@
         <v>139</v>
       </c>
       <c r="S19" s="4">
-        <f>PRODUCT(Q19,R19)</f>
+        <f t="shared" si="0"/>
         <v>6651.6715140999995</v>
       </c>
       <c r="T19">
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>22</v>
       </c>
@@ -2304,14 +2304,14 @@
         <v>57</v>
       </c>
       <c r="S20" s="4">
-        <f>PRODUCT(Q20,R20)</f>
+        <f t="shared" si="0"/>
         <v>6777.4759932000006</v>
       </c>
       <c r="T20">
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>24</v>
       </c>
@@ -2367,14 +2367,14 @@
         <v>57</v>
       </c>
       <c r="S21" s="4">
-        <f>PRODUCT(Q21,R21)</f>
+        <f t="shared" si="0"/>
         <v>6788.5368431999996</v>
       </c>
       <c r="T21">
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>16</v>
       </c>
@@ -2430,14 +2430,14 @@
         <v>224</v>
       </c>
       <c r="S22" s="4">
-        <f>PRODUCT(Q22,R22)</f>
+        <f t="shared" si="0"/>
         <v>6799.2015750400005</v>
       </c>
       <c r="T22">
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>24</v>
       </c>
@@ -2493,14 +2493,14 @@
         <v>152</v>
       </c>
       <c r="S23" s="4">
-        <f>PRODUCT(Q23,R23)</f>
+        <f t="shared" si="0"/>
         <v>6857.0575692000002</v>
       </c>
       <c r="T23">
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -2556,14 +2556,14 @@
         <v>57</v>
       </c>
       <c r="S24" s="4">
-        <f>PRODUCT(Q24,R24)</f>
+        <f t="shared" si="0"/>
         <v>6889.1085494999998</v>
       </c>
       <c r="T24">
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -2619,14 +2619,14 @@
         <v>139</v>
       </c>
       <c r="S25" s="4">
-        <f>PRODUCT(Q25,R25)</f>
+        <f t="shared" si="0"/>
         <v>6896.8310127000004</v>
       </c>
       <c r="T25">
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>22</v>
       </c>
@@ -2682,14 +2682,14 @@
         <v>57</v>
       </c>
       <c r="S26" s="4">
-        <f>PRODUCT(Q26,R26)</f>
+        <f t="shared" si="0"/>
         <v>6955.6365954000003</v>
       </c>
       <c r="T26">
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>22</v>
       </c>
@@ -2745,14 +2745,14 @@
         <v>117</v>
       </c>
       <c r="S27" s="4">
-        <f>PRODUCT(Q27,R27)</f>
+        <f t="shared" si="0"/>
         <v>6997.2167222099997</v>
       </c>
       <c r="T27">
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>24</v>
       </c>
@@ -2808,14 +2808,14 @@
         <v>152</v>
       </c>
       <c r="S28" s="4">
-        <f>PRODUCT(Q28,R28)</f>
+        <f t="shared" si="0"/>
         <v>7129.4529980799998</v>
       </c>
       <c r="T28">
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>16</v>
       </c>
@@ -2871,14 +2871,14 @@
         <v>113</v>
       </c>
       <c r="S29" s="4">
-        <f>PRODUCT(Q29,R29)</f>
+        <f t="shared" si="0"/>
         <v>7139.44308086</v>
       </c>
       <c r="T29">
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>23</v>
       </c>
@@ -2934,14 +2934,14 @@
         <v>57</v>
       </c>
       <c r="S30" s="4">
-        <f>PRODUCT(Q30,R30)</f>
+        <f t="shared" si="0"/>
         <v>7153.5183026999994</v>
       </c>
       <c r="T30">
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>22</v>
       </c>
@@ -2997,14 +2997,14 @@
         <v>139</v>
       </c>
       <c r="S31" s="4">
-        <f>PRODUCT(Q31,R31)</f>
+        <f t="shared" si="0"/>
         <v>7233.7874026100008</v>
       </c>
       <c r="T31">
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>23</v>
       </c>
@@ -3060,14 +3060,14 @@
         <v>139</v>
       </c>
       <c r="S32" s="4">
-        <f>PRODUCT(Q32,R32)</f>
+        <f t="shared" si="0"/>
         <v>7274.5618155100001</v>
       </c>
       <c r="T32">
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>16</v>
       </c>
@@ -3123,14 +3123,14 @@
         <v>182</v>
       </c>
       <c r="S33" s="4">
-        <f>PRODUCT(Q33,R33)</f>
+        <f t="shared" si="0"/>
         <v>7399.0111741000001</v>
       </c>
       <c r="T33">
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>24</v>
       </c>
@@ -3186,14 +3186,14 @@
         <v>57</v>
       </c>
       <c r="S34" s="4">
-        <f>PRODUCT(Q34,R34)</f>
+        <f t="shared" si="0"/>
         <v>7462.5917396999994</v>
       </c>
       <c r="T34">
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>24</v>
       </c>
@@ -3249,14 +3249,14 @@
         <v>152</v>
       </c>
       <c r="S35" s="4">
-        <f>PRODUCT(Q35,R35)</f>
+        <f t="shared" si="0"/>
         <v>7468.2744759200004</v>
       </c>
       <c r="T35">
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>22</v>
       </c>
@@ -3312,14 +3312,14 @@
         <v>57</v>
       </c>
       <c r="S36" s="4">
-        <f>PRODUCT(Q36,R36)</f>
+        <f t="shared" si="0"/>
         <v>7476.6461841</v>
       </c>
       <c r="T36">
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>16</v>
       </c>
@@ -3375,14 +3375,14 @@
         <v>224</v>
       </c>
       <c r="S37" s="4">
-        <f>PRODUCT(Q37,R37)</f>
+        <f t="shared" si="0"/>
         <v>7516.5617251200001</v>
       </c>
       <c r="T37">
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>22</v>
       </c>
@@ -3438,14 +3438,14 @@
         <v>117</v>
       </c>
       <c r="S38" s="4">
-        <f>PRODUCT(Q38,R38)</f>
+        <f t="shared" si="0"/>
         <v>7596.5830749900006</v>
       </c>
       <c r="T38">
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>24</v>
       </c>
@@ -3501,14 +3501,14 @@
         <v>57</v>
       </c>
       <c r="S39" s="4">
-        <f>PRODUCT(Q39,R39)</f>
+        <f t="shared" si="0"/>
         <v>7699.1853047999994</v>
       </c>
       <c r="T39">
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>22</v>
       </c>
@@ -3564,14 +3564,14 @@
         <v>117</v>
       </c>
       <c r="S40" s="4">
-        <f>PRODUCT(Q40,R40)</f>
+        <f t="shared" si="0"/>
         <v>7740.3908438999997</v>
       </c>
       <c r="T40">
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>16</v>
       </c>
@@ -3627,14 +3627,14 @@
         <v>224</v>
       </c>
       <c r="S41" s="4">
-        <f>PRODUCT(Q41,R41)</f>
+        <f t="shared" si="0"/>
         <v>7792.2257503999999</v>
       </c>
       <c r="T41">
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>22</v>
       </c>
@@ -3690,14 +3690,14 @@
         <v>139</v>
       </c>
       <c r="S42" s="4">
-        <f>PRODUCT(Q42,R42)</f>
+        <f t="shared" si="0"/>
         <v>7859.4977846700003</v>
       </c>
       <c r="T42">
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>23</v>
       </c>
@@ -3753,14 +3753,14 @@
         <v>57</v>
       </c>
       <c r="S43" s="4">
-        <f>PRODUCT(Q43,R43)</f>
+        <f t="shared" si="0"/>
         <v>7913.3058389999997</v>
       </c>
       <c r="T43">
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>24</v>
       </c>
@@ -3816,14 +3816,14 @@
         <v>139</v>
       </c>
       <c r="S44" s="4">
-        <f>PRODUCT(Q44,R44)</f>
+        <f t="shared" si="0"/>
         <v>7996.1708537800005</v>
       </c>
       <c r="T44">
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>23</v>
       </c>
@@ -3879,14 +3879,14 @@
         <v>139</v>
       </c>
       <c r="S45" s="4">
-        <f>PRODUCT(Q45,R45)</f>
+        <f t="shared" si="0"/>
         <v>8002.8171916000001</v>
       </c>
       <c r="T45">
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>22</v>
       </c>
@@ -3942,14 +3942,14 @@
         <v>139</v>
       </c>
       <c r="S46" s="4">
-        <f>PRODUCT(Q46,R46)</f>
+        <f t="shared" si="0"/>
         <v>8005.1321128900008</v>
       </c>
       <c r="T46">
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>24</v>
       </c>
@@ -4005,14 +4005,14 @@
         <v>57</v>
       </c>
       <c r="S47" s="4">
-        <f>PRODUCT(Q47,R47)</f>
+        <f t="shared" si="0"/>
         <v>8057.7959085000011</v>
       </c>
       <c r="T47">
         <v>3</v>
       </c>
     </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>16</v>
       </c>
@@ -4068,14 +4068,14 @@
         <v>113</v>
       </c>
       <c r="S48" s="4">
-        <f>PRODUCT(Q48,R48)</f>
+        <f t="shared" si="0"/>
         <v>8076.55539176</v>
       </c>
       <c r="T48">
         <v>3</v>
       </c>
     </row>
-    <row r="49" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>22</v>
       </c>
@@ -4131,14 +4131,14 @@
         <v>57</v>
       </c>
       <c r="S49" s="4">
-        <f>PRODUCT(Q49,R49)</f>
+        <f t="shared" si="0"/>
         <v>8106.5298711000005</v>
       </c>
       <c r="T49">
         <v>3</v>
       </c>
     </row>
-    <row r="50" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>16</v>
       </c>
@@ -4194,14 +4194,14 @@
         <v>224</v>
       </c>
       <c r="S50" s="4">
-        <f>PRODUCT(Q50,R50)</f>
+        <f t="shared" si="0"/>
         <v>8129.8017180799998</v>
       </c>
       <c r="T50">
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>23</v>
       </c>
@@ -4257,14 +4257,14 @@
         <v>57</v>
       </c>
       <c r="S51" s="4">
-        <f>PRODUCT(Q51,R51)</f>
+        <f t="shared" si="0"/>
         <v>8220.3112875000006</v>
       </c>
       <c r="T51">
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>24</v>
       </c>
@@ -4320,14 +4320,14 @@
         <v>152</v>
       </c>
       <c r="S52" s="4">
-        <f>PRODUCT(Q52,R52)</f>
+        <f t="shared" si="0"/>
         <v>8223.34244984</v>
       </c>
       <c r="T52">
         <v>2</v>
       </c>
     </row>
-    <row r="53" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>23</v>
       </c>
@@ -4383,14 +4383,14 @@
         <v>139</v>
       </c>
       <c r="S53" s="4">
-        <f>PRODUCT(Q53,R53)</f>
+        <f t="shared" si="0"/>
         <v>8250.2916100999992</v>
       </c>
       <c r="T53">
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>16</v>
       </c>
@@ -4446,14 +4446,14 @@
         <v>182</v>
       </c>
       <c r="S54" s="4">
-        <f>PRODUCT(Q54,R54)</f>
+        <f t="shared" si="0"/>
         <v>8274.5740440999998</v>
       </c>
       <c r="T54">
         <v>3</v>
       </c>
     </row>
-    <row r="55" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>22</v>
       </c>
@@ -4509,14 +4509,14 @@
         <v>57</v>
       </c>
       <c r="S55" s="4">
-        <f>PRODUCT(Q55,R55)</f>
+        <f t="shared" si="0"/>
         <v>8284.6904790000008</v>
       </c>
       <c r="T55">
         <v>3</v>
       </c>
     </row>
-    <row r="56" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>22</v>
       </c>
@@ -4572,14 +4572,14 @@
         <v>117</v>
       </c>
       <c r="S56" s="4">
-        <f>PRODUCT(Q56,R56)</f>
+        <f t="shared" si="0"/>
         <v>8333.3658107699994</v>
       </c>
       <c r="T56">
         <v>3</v>
       </c>
     </row>
-    <row r="57" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>23</v>
       </c>
@@ -4635,14 +4635,14 @@
         <v>57</v>
       </c>
       <c r="S57" s="4">
-        <f>PRODUCT(Q57,R57)</f>
+        <f t="shared" si="0"/>
         <v>8422.7773736999989</v>
       </c>
       <c r="T57">
         <v>3</v>
       </c>
     </row>
-    <row r="58" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>16</v>
       </c>
@@ -4698,14 +4698,14 @@
         <v>113</v>
       </c>
       <c r="S58" s="4">
-        <f>PRODUCT(Q58,R58)</f>
+        <f t="shared" si="0"/>
         <v>8442.3007967600006</v>
       </c>
       <c r="T58">
         <v>2</v>
       </c>
     </row>
-    <row r="59" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>24</v>
       </c>
@@ -4761,14 +4761,14 @@
         <v>152</v>
       </c>
       <c r="S59" s="4">
-        <f>PRODUCT(Q59,R59)</f>
+        <f t="shared" si="0"/>
         <v>8495.7378057599999</v>
       </c>
       <c r="T59">
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>23</v>
       </c>
@@ -4824,14 +4824,14 @@
         <v>117</v>
       </c>
       <c r="S60" s="4">
-        <f>PRODUCT(Q60,R60)</f>
+        <f t="shared" si="0"/>
         <v>8509.5222474599996</v>
       </c>
       <c r="T60">
         <v>3</v>
       </c>
     </row>
-    <row r="61" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>22</v>
       </c>
@@ -4887,14 +4887,14 @@
         <v>139</v>
       </c>
       <c r="S61" s="4">
-        <f>PRODUCT(Q61,R61)</f>
+        <f t="shared" si="0"/>
         <v>8525.3041943000007</v>
       </c>
       <c r="T61">
         <v>3</v>
       </c>
     </row>
-    <row r="62" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>23</v>
       </c>
@@ -4950,14 +4950,14 @@
         <v>139</v>
       </c>
       <c r="S62" s="4">
-        <f>PRODUCT(Q62,R62)</f>
+        <f t="shared" si="0"/>
         <v>8566.078607200001</v>
       </c>
       <c r="T62">
         <v>3</v>
       </c>
     </row>
-    <row r="63" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>16</v>
       </c>
@@ -5013,14 +5013,14 @@
         <v>113</v>
       </c>
       <c r="S63" s="4">
-        <f>PRODUCT(Q63,R63)</f>
+        <f t="shared" si="0"/>
         <v>8622.9649978800007</v>
       </c>
       <c r="T63">
         <v>3</v>
       </c>
     </row>
-    <row r="64" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>16</v>
       </c>
@@ -5076,14 +5076,14 @@
         <v>182</v>
       </c>
       <c r="S64" s="4">
-        <f>PRODUCT(Q64,R64)</f>
+        <f t="shared" si="0"/>
         <v>8672.4336917399996</v>
       </c>
       <c r="T64">
         <v>3</v>
       </c>
     </row>
-    <row r="65" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>16</v>
       </c>
@@ -5139,14 +5139,14 @@
         <v>182</v>
       </c>
       <c r="S65" s="4">
-        <f>PRODUCT(Q65,R65)</f>
+        <f t="shared" si="0"/>
         <v>8740.2389074000002</v>
       </c>
       <c r="T65">
         <v>2</v>
       </c>
     </row>
-    <row r="66" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>24</v>
       </c>
@@ -5202,14 +5202,14 @@
         <v>152</v>
       </c>
       <c r="S66" s="4">
-        <f>PRODUCT(Q66,R66)</f>
+        <f t="shared" ref="S66:S129" si="1">PRODUCT(Q66,R66)</f>
         <v>8772.615579360001</v>
       </c>
       <c r="T66">
         <v>3</v>
       </c>
     </row>
-    <row r="67" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>24</v>
       </c>
@@ -5265,14 +5265,14 @@
         <v>57</v>
       </c>
       <c r="S67" s="4">
-        <f>PRODUCT(Q67,R67)</f>
+        <f t="shared" si="1"/>
         <v>8791.6456118999995</v>
       </c>
       <c r="T67">
         <v>3</v>
       </c>
     </row>
-    <row r="68" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>16</v>
       </c>
@@ -5328,14 +5328,14 @@
         <v>224</v>
       </c>
       <c r="S68" s="4">
-        <f>PRODUCT(Q68,R68)</f>
+        <f t="shared" si="1"/>
         <v>8907.0494441600003</v>
       </c>
       <c r="T68">
         <v>2</v>
       </c>
     </row>
-    <row r="69" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>22</v>
       </c>
@@ -5391,14 +5391,14 @@
         <v>57</v>
       </c>
       <c r="S69" s="4">
-        <f>PRODUCT(Q69,R69)</f>
+        <f t="shared" si="1"/>
         <v>8945.7762908999994</v>
       </c>
       <c r="T69">
         <v>4</v>
       </c>
     </row>
-    <row r="70" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>22</v>
       </c>
@@ -5454,14 +5454,14 @@
         <v>117</v>
       </c>
       <c r="S70" s="4">
-        <f>PRODUCT(Q70,R70)</f>
+        <f t="shared" si="1"/>
         <v>8992.5269768100006</v>
       </c>
       <c r="T70">
         <v>3</v>
       </c>
     </row>
-    <row r="71" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>24</v>
       </c>
@@ -5517,14 +5517,14 @@
         <v>57</v>
       </c>
       <c r="S71" s="4">
-        <f>PRODUCT(Q71,R71)</f>
+        <f t="shared" si="1"/>
         <v>9028.239188399999</v>
       </c>
       <c r="T71">
         <v>3</v>
       </c>
     </row>
-    <row r="72" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>22</v>
       </c>
@@ -5580,14 +5580,14 @@
         <v>57</v>
       </c>
       <c r="S72" s="4">
-        <f>PRODUCT(Q72,R72)</f>
+        <f t="shared" si="1"/>
         <v>9098.6773145999996</v>
       </c>
       <c r="T72">
         <v>3</v>
       </c>
     </row>
-    <row r="73" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>24</v>
       </c>
@@ -5643,14 +5643,14 @@
         <v>139</v>
       </c>
       <c r="S73" s="4">
-        <f>PRODUCT(Q73,R73)</f>
+        <f t="shared" si="1"/>
         <v>9104.1291577299999</v>
       </c>
       <c r="T73">
         <v>3</v>
       </c>
     </row>
-    <row r="74" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>22</v>
       </c>
@@ -5706,14 +5706,14 @@
         <v>117</v>
       </c>
       <c r="S74" s="4">
-        <f>PRODUCT(Q74,R74)</f>
+        <f t="shared" si="1"/>
         <v>9136.3348018800007</v>
       </c>
       <c r="T74">
         <v>3</v>
       </c>
     </row>
-    <row r="75" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>16</v>
       </c>
@@ -5769,14 +5769,14 @@
         <v>224</v>
       </c>
       <c r="S75" s="4">
-        <f>PRODUCT(Q75,R75)</f>
+        <f t="shared" si="1"/>
         <v>9182.71352544</v>
       </c>
       <c r="T75">
         <v>2</v>
       </c>
     </row>
-    <row r="76" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>22</v>
       </c>
@@ -5832,14 +5832,14 @@
         <v>139</v>
       </c>
       <c r="S76" s="4">
-        <f>PRODUCT(Q76,R76)</f>
+        <f t="shared" si="1"/>
         <v>9210.809373959999</v>
       </c>
       <c r="T76">
         <v>3</v>
       </c>
     </row>
-    <row r="77" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>23</v>
       </c>
@@ -5895,14 +5895,14 @@
         <v>57</v>
       </c>
       <c r="S77" s="4">
-        <f>PRODUCT(Q77,R77)</f>
+        <f t="shared" si="1"/>
         <v>9242.3597111999989</v>
       </c>
       <c r="T77">
         <v>3</v>
       </c>
     </row>
-    <row r="78" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>24</v>
       </c>
@@ -5958,14 +5958,14 @@
         <v>139</v>
       </c>
       <c r="S78" s="4">
-        <f>PRODUCT(Q78,R78)</f>
+        <f t="shared" si="1"/>
         <v>9289.7439753300005</v>
       </c>
       <c r="T78">
         <v>2</v>
       </c>
     </row>
-    <row r="79" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>24</v>
       </c>
@@ -6021,14 +6021,14 @@
         <v>57</v>
       </c>
       <c r="S79" s="4">
-        <f>PRODUCT(Q79,R79)</f>
+        <f t="shared" si="1"/>
         <v>9325.8629784000004</v>
       </c>
       <c r="T79">
         <v>4</v>
       </c>
     </row>
-    <row r="80" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>23</v>
       </c>
@@ -6084,14 +6084,14 @@
         <v>139</v>
       </c>
       <c r="S80" s="4">
-        <f>PRODUCT(Q80,R80)</f>
+        <f t="shared" si="1"/>
         <v>9354.1287808900015</v>
       </c>
       <c r="T80">
         <v>3</v>
       </c>
     </row>
-    <row r="81" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>22</v>
       </c>
@@ -6147,14 +6147,14 @@
         <v>139</v>
       </c>
       <c r="S81" s="4">
-        <f>PRODUCT(Q81,R81)</f>
+        <f t="shared" si="1"/>
         <v>9356.4436729900008</v>
       </c>
       <c r="T81">
         <v>3</v>
       </c>
     </row>
-    <row r="82" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>16</v>
       </c>
@@ -6210,14 +6210,14 @@
         <v>113</v>
       </c>
       <c r="S82" s="4">
-        <f>PRODUCT(Q82,R82)</f>
+        <f t="shared" si="1"/>
         <v>9439.3006634699996</v>
       </c>
       <c r="T82">
         <v>2</v>
       </c>
     </row>
-    <row r="83" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>16</v>
       </c>
@@ -6273,14 +6273,14 @@
         <v>224</v>
       </c>
       <c r="S83" s="4">
-        <f>PRODUCT(Q83,R83)</f>
+        <f t="shared" si="1"/>
         <v>9458.34550304</v>
       </c>
       <c r="T83">
         <v>3</v>
       </c>
     </row>
-    <row r="84" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>23</v>
       </c>
@@ -6336,14 +6336,14 @@
         <v>57</v>
       </c>
       <c r="S84" s="4">
-        <f>PRODUCT(Q84,R84)</f>
+        <f t="shared" si="1"/>
         <v>9549.3651711000002</v>
       </c>
       <c r="T84">
         <v>3</v>
       </c>
     </row>
-    <row r="85" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>24</v>
       </c>
@@ -6399,14 +6399,14 @@
         <v>152</v>
       </c>
       <c r="S85" s="4">
-        <f>PRODUCT(Q85,R85)</f>
+        <f t="shared" si="1"/>
         <v>9587.4783514400006</v>
       </c>
       <c r="T85">
         <v>3</v>
       </c>
     </row>
-    <row r="86" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>23</v>
       </c>
@@ -6462,14 +6462,14 @@
         <v>139</v>
       </c>
       <c r="S86" s="4">
-        <f>PRODUCT(Q86,R86)</f>
+        <f t="shared" si="1"/>
         <v>9601.603171589999</v>
       </c>
       <c r="T86">
         <v>3</v>
       </c>
     </row>
-    <row r="87" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>16</v>
       </c>
@@ -6525,14 +6525,14 @@
         <v>182</v>
       </c>
       <c r="S87" s="4">
-        <f>PRODUCT(Q87,R87)</f>
+        <f t="shared" si="1"/>
         <v>9676.0653971800002</v>
       </c>
       <c r="T87">
         <v>2</v>
       </c>
     </row>
-    <row r="88" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>22</v>
       </c>
@@ -6588,14 +6588,14 @@
         <v>57</v>
       </c>
       <c r="S88" s="4">
-        <f>PRODUCT(Q88,R88)</f>
+        <f t="shared" si="1"/>
         <v>9677.3006792999986</v>
       </c>
       <c r="T88">
         <v>4</v>
       </c>
     </row>
-    <row r="89" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>24</v>
       </c>
@@ -6651,14 +6651,14 @@
         <v>139</v>
       </c>
       <c r="S89" s="4">
-        <f>PRODUCT(Q89,R89)</f>
+        <f t="shared" si="1"/>
         <v>9711.5015769799993</v>
       </c>
       <c r="T89">
         <v>3</v>
       </c>
     </row>
-    <row r="90" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>16</v>
       </c>
@@ -6714,14 +6714,14 @@
         <v>113</v>
       </c>
       <c r="S90" s="4">
-        <f>PRODUCT(Q90,R90)</f>
+        <f t="shared" si="1"/>
         <v>9743.1022957299992</v>
       </c>
       <c r="T90">
         <v>3</v>
       </c>
     </row>
-    <row r="91" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>23</v>
       </c>
@@ -6777,14 +6777,14 @@
         <v>117</v>
       </c>
       <c r="S91" s="4">
-        <f>PRODUCT(Q91,R91)</f>
+        <f t="shared" si="1"/>
         <v>9755.079072569999</v>
       </c>
       <c r="T91">
         <v>3</v>
       </c>
     </row>
-    <row r="92" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>22</v>
       </c>
@@ -6840,14 +6840,14 @@
         <v>139</v>
       </c>
       <c r="S92" s="4">
-        <f>PRODUCT(Q92,R92)</f>
+        <f t="shared" si="1"/>
         <v>9815.629170799999</v>
       </c>
       <c r="T92">
         <v>4</v>
       </c>
     </row>
-    <row r="93" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>23</v>
       </c>
@@ -6903,14 +6903,14 @@
         <v>117</v>
       </c>
       <c r="S93" s="4">
-        <f>PRODUCT(Q93,R93)</f>
+        <f t="shared" si="1"/>
         <v>9831.6899846100005</v>
       </c>
       <c r="T93">
         <v>4</v>
       </c>
     </row>
-    <row r="94" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>23</v>
       </c>
@@ -6966,14 +6966,14 @@
         <v>117</v>
       </c>
       <c r="S94" s="4">
-        <f>PRODUCT(Q94,R94)</f>
+        <f t="shared" si="1"/>
         <v>9847.7275337999999</v>
       </c>
       <c r="T94">
         <v>2</v>
       </c>
     </row>
-    <row r="95" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>23</v>
       </c>
@@ -7029,14 +7029,14 @@
         <v>139</v>
       </c>
       <c r="S95" s="4">
-        <f>PRODUCT(Q95,R95)</f>
+        <f t="shared" si="1"/>
         <v>9856.4035836999992</v>
       </c>
       <c r="T95">
         <v>4</v>
       </c>
     </row>
-    <row r="96" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>24</v>
       </c>
@@ -7092,14 +7092,14 @@
         <v>152</v>
       </c>
       <c r="S96" s="4">
-        <f>PRODUCT(Q96,R96)</f>
+        <f t="shared" si="1"/>
         <v>9859.8736784800003</v>
       </c>
       <c r="T96">
         <v>3</v>
       </c>
     </row>
-    <row r="97" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>22</v>
       </c>
@@ -7155,14 +7155,14 @@
         <v>57</v>
       </c>
       <c r="S97" s="4">
-        <f>PRODUCT(Q97,R97)</f>
+        <f t="shared" si="1"/>
         <v>9889.1389734000004</v>
       </c>
       <c r="T97">
         <v>4</v>
       </c>
     </row>
-    <row r="98" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>16</v>
       </c>
@@ -7218,14 +7218,14 @@
         <v>113</v>
       </c>
       <c r="S98" s="4">
-        <f>PRODUCT(Q98,R98)</f>
+        <f t="shared" si="1"/>
         <v>9985.71026394</v>
       </c>
       <c r="T98">
         <v>2</v>
       </c>
     </row>
-    <row r="99" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>22</v>
       </c>
@@ -7281,14 +7281,14 @@
         <v>117</v>
       </c>
       <c r="S99" s="4">
-        <f>PRODUCT(Q99,R99)</f>
+        <f t="shared" si="1"/>
         <v>9995.0696117999996</v>
       </c>
       <c r="T99">
         <v>4</v>
       </c>
     </row>
-    <row r="100" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>23</v>
       </c>
@@ -7344,14 +7344,14 @@
         <v>57</v>
       </c>
       <c r="S100" s="4">
-        <f>PRODUCT(Q100,R100)</f>
+        <f t="shared" si="1"/>
         <v>10011.882431399999</v>
       </c>
       <c r="T100">
         <v>4</v>
       </c>
     </row>
-    <row r="101" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>22</v>
       </c>
@@ -7407,14 +7407,14 @@
         <v>57</v>
       </c>
       <c r="S101" s="4">
-        <f>PRODUCT(Q101,R101)</f>
+        <f t="shared" si="1"/>
         <v>10039.8315207</v>
       </c>
       <c r="T101">
         <v>3</v>
       </c>
     </row>
-    <row r="102" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>16</v>
       </c>
@@ -7470,14 +7470,14 @@
         <v>182</v>
       </c>
       <c r="S102" s="4">
-        <f>PRODUCT(Q102,R102)</f>
+        <f t="shared" si="1"/>
         <v>10073.925046640001</v>
       </c>
       <c r="T102">
         <v>2</v>
       </c>
     </row>
-    <row r="103" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>24</v>
       </c>
@@ -7533,14 +7533,14 @@
         <v>152</v>
       </c>
       <c r="S103" s="4">
-        <f>PRODUCT(Q103,R103)</f>
+        <f t="shared" si="1"/>
         <v>10075.764666879999</v>
       </c>
       <c r="T103">
         <v>4</v>
       </c>
     </row>
-    <row r="104" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>16</v>
       </c>
@@ -7596,14 +7596,14 @@
         <v>182</v>
       </c>
       <c r="S104" s="4">
-        <f>PRODUCT(Q104,R104)</f>
+        <f t="shared" si="1"/>
         <v>10078.38351702</v>
       </c>
       <c r="T104">
         <v>3</v>
       </c>
     </row>
-    <row r="105" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>24</v>
       </c>
@@ -7659,14 +7659,14 @@
         <v>57</v>
       </c>
       <c r="S105" s="4">
-        <f>PRODUCT(Q105,R105)</f>
+        <f t="shared" si="1"/>
         <v>10119.4536864</v>
       </c>
       <c r="T105">
         <v>4</v>
       </c>
     </row>
-    <row r="106" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>16</v>
       </c>
@@ -7722,14 +7722,14 @@
         <v>224</v>
       </c>
       <c r="S106" s="4">
-        <f>PRODUCT(Q106,R106)</f>
+        <f t="shared" si="1"/>
         <v>10295.388010879999</v>
       </c>
       <c r="T106">
         <v>3</v>
       </c>
     </row>
-    <row r="107" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>24</v>
       </c>
@@ -7785,14 +7785,14 @@
         <v>57</v>
       </c>
       <c r="S107" s="4">
-        <f>PRODUCT(Q107,R107)</f>
+        <f t="shared" si="1"/>
         <v>10356.047268599999</v>
       </c>
       <c r="T107">
         <v>4</v>
       </c>
     </row>
-    <row r="108" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>24</v>
       </c>
@@ -7848,14 +7848,14 @@
         <v>139</v>
       </c>
       <c r="S108" s="4">
-        <f>PRODUCT(Q108,R108)</f>
+        <f t="shared" si="1"/>
         <v>10457.58982741</v>
       </c>
       <c r="T108">
         <v>2</v>
       </c>
     </row>
-    <row r="109" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>22</v>
       </c>
@@ -7911,14 +7911,14 @@
         <v>57</v>
       </c>
       <c r="S109" s="4">
-        <f>PRODUCT(Q109,R109)</f>
+        <f t="shared" si="1"/>
         <v>10458.656411400001</v>
       </c>
       <c r="T109">
         <v>2</v>
       </c>
     </row>
-    <row r="110" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>23</v>
       </c>
@@ -7974,14 +7974,14 @@
         <v>117</v>
       </c>
       <c r="S110" s="4">
-        <f>PRODUCT(Q110,R110)</f>
+        <f t="shared" si="1"/>
         <v>10471.210929270001</v>
       </c>
       <c r="T110">
         <v>3</v>
       </c>
     </row>
-    <row r="111" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>22</v>
       </c>
@@ -8037,14 +8037,14 @@
         <v>57</v>
       </c>
       <c r="S111" s="4">
-        <f>PRODUCT(Q111,R111)</f>
+        <f t="shared" si="1"/>
         <v>10543.1509656</v>
       </c>
       <c r="T111">
         <v>3</v>
       </c>
     </row>
-    <row r="112" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>22</v>
       </c>
@@ -8100,14 +8100,14 @@
         <v>139</v>
       </c>
       <c r="S112" s="4">
-        <f>PRODUCT(Q112,R112)</f>
+        <f t="shared" si="1"/>
         <v>10560.875334209999</v>
       </c>
       <c r="T112">
         <v>4</v>
       </c>
     </row>
-    <row r="113" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>16</v>
       </c>
@@ -8163,14 +8163,14 @@
         <v>224</v>
       </c>
       <c r="S113" s="4">
-        <f>PRODUCT(Q113,R113)</f>
+        <f t="shared" si="1"/>
         <v>10571.052116800001</v>
       </c>
       <c r="T113">
         <v>3</v>
       </c>
     </row>
-    <row r="114" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>24</v>
       </c>
@@ -8226,14 +8226,14 @@
         <v>139</v>
       </c>
       <c r="S114" s="4">
-        <f>PRODUCT(Q114,R114)</f>
+        <f t="shared" si="1"/>
         <v>10581.26076702</v>
       </c>
       <c r="T114">
         <v>3</v>
       </c>
     </row>
-    <row r="115" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>23</v>
       </c>
@@ -8289,14 +8289,14 @@
         <v>117</v>
       </c>
       <c r="S115" s="4">
-        <f>PRODUCT(Q115,R115)</f>
+        <f t="shared" si="1"/>
         <v>10633.86943047</v>
       </c>
       <c r="T115">
         <v>4</v>
       </c>
     </row>
-    <row r="116" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>23</v>
       </c>
@@ -8352,14 +8352,14 @@
         <v>139</v>
       </c>
       <c r="S116" s="4">
-        <f>PRODUCT(Q116,R116)</f>
+        <f t="shared" si="1"/>
         <v>10704.194741140001</v>
       </c>
       <c r="T116">
         <v>4</v>
       </c>
     </row>
-    <row r="117" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>22</v>
       </c>
@@ -8415,14 +8415,14 @@
         <v>139</v>
       </c>
       <c r="S117" s="4">
-        <f>PRODUCT(Q117,R117)</f>
+        <f t="shared" si="1"/>
         <v>10706.509651310002</v>
       </c>
       <c r="T117">
         <v>4</v>
       </c>
     </row>
-    <row r="118" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>22</v>
       </c>
@@ -8478,14 +8478,14 @@
         <v>117</v>
       </c>
       <c r="S118" s="4">
-        <f>PRODUCT(Q118,R118)</f>
+        <f t="shared" si="1"/>
         <v>10760.80279482</v>
       </c>
       <c r="T118">
         <v>4</v>
       </c>
     </row>
-    <row r="119" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>16</v>
       </c>
@@ -8541,14 +8541,14 @@
         <v>224</v>
       </c>
       <c r="S119" s="4">
-        <f>PRODUCT(Q119,R119)</f>
+        <f t="shared" si="1"/>
         <v>10785.697596800001</v>
       </c>
       <c r="T119">
         <v>4</v>
       </c>
     </row>
-    <row r="120" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>16</v>
       </c>
@@ -8604,14 +8604,14 @@
         <v>113</v>
       </c>
       <c r="S120" s="4">
-        <f>PRODUCT(Q120,R120)</f>
+        <f t="shared" si="1"/>
         <v>10799.896976889999</v>
       </c>
       <c r="T120">
         <v>3</v>
       </c>
     </row>
-    <row r="121" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>23</v>
       </c>
@@ -8667,14 +8667,14 @@
         <v>117</v>
       </c>
       <c r="S121" s="4">
-        <f>PRODUCT(Q121,R121)</f>
+        <f t="shared" si="1"/>
         <v>10881.035505990001</v>
       </c>
       <c r="T121">
         <v>4</v>
       </c>
     </row>
-    <row r="122" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>23</v>
       </c>
@@ -8730,14 +8730,14 @@
         <v>57</v>
       </c>
       <c r="S122" s="4">
-        <f>PRODUCT(Q122,R122)</f>
+        <f t="shared" si="1"/>
         <v>10906.6865574</v>
       </c>
       <c r="T122">
         <v>4</v>
       </c>
     </row>
-    <row r="123" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>22</v>
       </c>
@@ -8793,14 +8793,14 @@
         <v>117</v>
       </c>
       <c r="S123" s="4">
-        <f>PRODUCT(Q123,R123)</f>
+        <f t="shared" si="1"/>
         <v>10942.204711229999</v>
       </c>
       <c r="T123">
         <v>4</v>
       </c>
     </row>
-    <row r="124" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>24</v>
       </c>
@@ -8856,14 +8856,14 @@
         <v>152</v>
       </c>
       <c r="S124" s="4">
-        <f>PRODUCT(Q124,R124)</f>
+        <f t="shared" si="1"/>
         <v>10950.368423040001</v>
       </c>
       <c r="T124">
         <v>4</v>
       </c>
     </row>
-    <row r="125" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>23</v>
       </c>
@@ -8919,14 +8919,14 @@
         <v>139</v>
       </c>
       <c r="S125" s="4">
-        <f>PRODUCT(Q125,R125)</f>
+        <f t="shared" si="1"/>
         <v>10951.669148519999</v>
       </c>
       <c r="T125">
         <v>4</v>
       </c>
     </row>
-    <row r="126" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>24</v>
       </c>
@@ -8982,14 +8982,14 @@
         <v>57</v>
       </c>
       <c r="S126" s="4">
-        <f>PRODUCT(Q126,R126)</f>
+        <f t="shared" si="1"/>
         <v>10990.789743899999</v>
       </c>
       <c r="T126">
         <v>3</v>
       </c>
     </row>
-    <row r="127" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>16</v>
       </c>
@@ -9045,14 +9045,14 @@
         <v>113</v>
       </c>
       <c r="S127" s="4">
-        <f>PRODUCT(Q127,R127)</f>
+        <f t="shared" si="1"/>
         <v>11042.71197353</v>
       </c>
       <c r="T127">
         <v>4</v>
       </c>
     </row>
-    <row r="128" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>24</v>
       </c>
@@ -9108,14 +9108,14 @@
         <v>139</v>
       </c>
       <c r="S128" s="4">
-        <f>PRODUCT(Q128,R128)</f>
+        <f t="shared" si="1"/>
         <v>11064.96217438</v>
       </c>
       <c r="T128">
         <v>2</v>
       </c>
     </row>
-    <row r="129" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>16</v>
       </c>
@@ -9171,14 +9171,14 @@
         <v>182</v>
       </c>
       <c r="S129" s="4">
-        <f>PRODUCT(Q129,R129)</f>
+        <f t="shared" si="1"/>
         <v>11074.334509420001</v>
       </c>
       <c r="T129">
         <v>3</v>
       </c>
     </row>
-    <row r="130" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>22</v>
       </c>
@@ -9234,14 +9234,14 @@
         <v>117</v>
       </c>
       <c r="S130" s="4">
-        <f>PRODUCT(Q130,R130)</f>
+        <f t="shared" ref="S130:S193" si="2">PRODUCT(Q130,R130)</f>
         <v>11094.3661023</v>
       </c>
       <c r="T130">
         <v>3</v>
       </c>
     </row>
-    <row r="131" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>23</v>
       </c>
@@ -9297,14 +9297,14 @@
         <v>117</v>
       </c>
       <c r="S131" s="4">
-        <f>PRODUCT(Q131,R131)</f>
+        <f t="shared" si="2"/>
         <v>11153.171915729999</v>
       </c>
       <c r="T131">
         <v>2</v>
       </c>
     </row>
-    <row r="132" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>23</v>
       </c>
@@ -9360,14 +9360,14 @@
         <v>117</v>
       </c>
       <c r="S132" s="4">
-        <f>PRODUCT(Q132,R132)</f>
+        <f t="shared" si="2"/>
         <v>11183.87662236</v>
       </c>
       <c r="T132">
         <v>3</v>
       </c>
     </row>
-    <row r="133" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>24</v>
       </c>
@@ -9423,14 +9423,14 @@
         <v>152</v>
       </c>
       <c r="S133" s="4">
-        <f>PRODUCT(Q133,R133)</f>
+        <f t="shared" si="2"/>
         <v>11222.763766799999</v>
       </c>
       <c r="T133">
         <v>4</v>
       </c>
     </row>
-    <row r="134" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>23</v>
       </c>
@@ -9486,14 +9486,14 @@
         <v>57</v>
       </c>
       <c r="S134" s="4">
-        <f>PRODUCT(Q134,R134)</f>
+        <f t="shared" si="2"/>
         <v>11267.2443951</v>
       </c>
       <c r="T134">
         <v>4</v>
       </c>
     </row>
-    <row r="135" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>16</v>
       </c>
@@ -9549,14 +9549,14 @@
         <v>113</v>
       </c>
       <c r="S135" s="4">
-        <f>PRODUCT(Q135,R135)</f>
+        <f t="shared" si="2"/>
         <v>11346.3066316</v>
       </c>
       <c r="T135">
         <v>3</v>
       </c>
     </row>
-    <row r="136" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>16</v>
       </c>
@@ -9612,14 +9612,14 @@
         <v>182</v>
       </c>
       <c r="S136" s="4">
-        <f>PRODUCT(Q136,R136)</f>
+        <f t="shared" si="2"/>
         <v>11414.737872720001</v>
       </c>
       <c r="T136">
         <v>4</v>
       </c>
     </row>
-    <row r="137" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>22</v>
       </c>
@@ -9675,14 +9675,14 @@
         <v>57</v>
       </c>
       <c r="S137" s="4">
-        <f>PRODUCT(Q137,R137)</f>
+        <f t="shared" si="2"/>
         <v>11467.815761399999</v>
       </c>
       <c r="T137">
         <v>2</v>
       </c>
     </row>
-    <row r="138" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>16</v>
       </c>
@@ -9738,14 +9738,14 @@
         <v>182</v>
       </c>
       <c r="S138" s="4">
-        <f>PRODUCT(Q138,R138)</f>
+        <f t="shared" si="2"/>
         <v>11472.194151600001</v>
       </c>
       <c r="T138">
         <v>3</v>
       </c>
     </row>
-    <row r="139" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>16</v>
       </c>
@@ -9801,14 +9801,14 @@
         <v>224</v>
       </c>
       <c r="S139" s="4">
-        <f>PRODUCT(Q139,R139)</f>
+        <f t="shared" si="2"/>
         <v>11682.48111968</v>
       </c>
       <c r="T139">
         <v>4</v>
       </c>
     </row>
-    <row r="140" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>22</v>
       </c>
@@ -9864,14 +9864,14 @@
         <v>139</v>
       </c>
       <c r="S140" s="4">
-        <f>PRODUCT(Q140,R140)</f>
+        <f t="shared" si="2"/>
         <v>11708.28116262</v>
       </c>
       <c r="T140">
         <v>3</v>
       </c>
     </row>
-    <row r="141" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>24</v>
       </c>
@@ -9927,14 +9927,14 @@
         <v>139</v>
       </c>
       <c r="S141" s="4">
-        <f>PRODUCT(Q141,R141)</f>
+        <f t="shared" si="2"/>
         <v>11808.901416699999</v>
       </c>
       <c r="T141">
         <v>3</v>
       </c>
     </row>
-    <row r="142" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>22</v>
       </c>
@@ -9990,14 +9990,14 @@
         <v>57</v>
       </c>
       <c r="S142" s="4">
-        <f>PRODUCT(Q142,R142)</f>
+        <f t="shared" si="2"/>
         <v>11814.981791100001</v>
       </c>
       <c r="T142">
         <v>3</v>
       </c>
     </row>
-    <row r="143" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>23</v>
       </c>
@@ -10053,14 +10053,14 @@
         <v>117</v>
       </c>
       <c r="S143" s="4">
-        <f>PRODUCT(Q143,R143)</f>
+        <f t="shared" si="2"/>
         <v>11869.303761900001</v>
       </c>
       <c r="T143">
         <v>2</v>
       </c>
     </row>
-    <row r="144" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>24</v>
       </c>
@@ -10116,14 +10116,14 @@
         <v>139</v>
       </c>
       <c r="S144" s="4">
-        <f>PRODUCT(Q144,R144)</f>
+        <f t="shared" si="2"/>
         <v>11871.58574352</v>
       </c>
       <c r="T144">
         <v>4</v>
       </c>
     </row>
-    <row r="145" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>23</v>
       </c>
@@ -10179,14 +10179,14 @@
         <v>139</v>
       </c>
       <c r="S145" s="4">
-        <f>PRODUCT(Q145,R145)</f>
+        <f t="shared" si="2"/>
         <v>11897.37682517</v>
       </c>
       <c r="T145">
         <v>3</v>
       </c>
     </row>
-    <row r="146" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>16</v>
       </c>
@@ -10242,14 +10242,14 @@
         <v>224</v>
       </c>
       <c r="S146" s="4">
-        <f>PRODUCT(Q146,R146)</f>
+        <f t="shared" si="2"/>
         <v>11958.14519648</v>
       </c>
       <c r="T146">
         <v>4</v>
       </c>
     </row>
-    <row r="147" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>22</v>
       </c>
@@ -10305,14 +10305,14 @@
         <v>57</v>
       </c>
       <c r="S147" s="4">
-        <f>PRODUCT(Q147,R147)</f>
+        <f t="shared" si="2"/>
         <v>11971.1351493</v>
       </c>
       <c r="T147">
         <v>2</v>
       </c>
     </row>
-    <row r="148" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>23</v>
       </c>
@@ -10368,14 +10368,14 @@
         <v>57</v>
       </c>
       <c r="S148" s="4">
-        <f>PRODUCT(Q148,R148)</f>
+        <f t="shared" si="2"/>
         <v>12006.2501361</v>
       </c>
       <c r="T148">
         <v>3</v>
       </c>
     </row>
-    <row r="149" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>24</v>
       </c>
@@ -10431,14 +10431,14 @@
         <v>57</v>
       </c>
       <c r="S149" s="4">
-        <f>PRODUCT(Q149,R149)</f>
+        <f t="shared" si="2"/>
         <v>12013.594933800001</v>
       </c>
       <c r="T149">
         <v>3</v>
       </c>
     </row>
-    <row r="150" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>22</v>
       </c>
@@ -10494,14 +10494,14 @@
         <v>117</v>
       </c>
       <c r="S150" s="4">
-        <f>PRODUCT(Q150,R150)</f>
+        <f t="shared" si="2"/>
         <v>12134.862125099999</v>
       </c>
       <c r="T150">
         <v>3</v>
       </c>
     </row>
-    <row r="151" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>16</v>
       </c>
@@ -10557,14 +10557,14 @@
         <v>113</v>
       </c>
       <c r="S151" s="4">
-        <f>PRODUCT(Q151,R151)</f>
+        <f t="shared" si="2"/>
         <v>12159.2476608</v>
       </c>
       <c r="T151">
         <v>4</v>
       </c>
     </row>
-    <row r="152" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>24</v>
       </c>
@@ -10620,14 +10620,14 @@
         <v>57</v>
       </c>
       <c r="S152" s="4">
-        <f>PRODUCT(Q152,R152)</f>
+        <f t="shared" si="2"/>
         <v>12350.7688464</v>
       </c>
       <c r="T152">
         <v>2</v>
       </c>
     </row>
-    <row r="153" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>24</v>
       </c>
@@ -10683,14 +10683,14 @@
         <v>152</v>
       </c>
       <c r="S153" s="4">
-        <f>PRODUCT(Q153,R153)</f>
+        <f t="shared" si="2"/>
         <v>12364.74156192</v>
       </c>
       <c r="T153">
         <v>3</v>
       </c>
     </row>
-    <row r="154" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>24</v>
       </c>
@@ -10746,14 +10746,14 @@
         <v>139</v>
       </c>
       <c r="S154" s="4">
-        <f>PRODUCT(Q154,R154)</f>
+        <f t="shared" si="2"/>
         <v>12416.273735870001</v>
       </c>
       <c r="T154">
         <v>3</v>
       </c>
     </row>
-    <row r="155" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>16</v>
       </c>
@@ -10809,14 +10809,14 @@
         <v>182</v>
       </c>
       <c r="S155" s="4">
-        <f>PRODUCT(Q155,R155)</f>
+        <f t="shared" si="2"/>
         <v>12470.732563380001</v>
       </c>
       <c r="T155">
         <v>4</v>
       </c>
     </row>
-    <row r="156" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>22</v>
       </c>
@@ -10872,14 +10872,14 @@
         <v>117</v>
       </c>
       <c r="S156" s="4">
-        <f>PRODUCT(Q156,R156)</f>
+        <f t="shared" si="2"/>
         <v>12545.528287499999</v>
       </c>
       <c r="T156">
         <v>3</v>
       </c>
     </row>
-    <row r="157" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>23</v>
       </c>
@@ -10935,14 +10935,14 @@
         <v>117</v>
       </c>
       <c r="S157" s="4">
-        <f>PRODUCT(Q157,R157)</f>
+        <f t="shared" si="2"/>
         <v>12549.1158117</v>
       </c>
       <c r="T157">
         <v>3</v>
       </c>
     </row>
-    <row r="158" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>22</v>
       </c>
@@ -10998,14 +10998,14 @@
         <v>117</v>
       </c>
       <c r="S158" s="4">
-        <f>PRODUCT(Q158,R158)</f>
+        <f t="shared" si="2"/>
         <v>12580.531119000001</v>
       </c>
       <c r="T158">
         <v>2</v>
       </c>
     </row>
-    <row r="159" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>24</v>
       </c>
@@ -11061,14 +11061,14 @@
         <v>57</v>
       </c>
       <c r="S159" s="4">
-        <f>PRODUCT(Q159,R159)</f>
+        <f t="shared" si="2"/>
         <v>12602.572616400001</v>
       </c>
       <c r="T159">
         <v>3</v>
       </c>
     </row>
-    <row r="160" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>16</v>
       </c>
@@ -11124,14 +11124,14 @@
         <v>113</v>
       </c>
       <c r="S160" s="4">
-        <f>PRODUCT(Q160,R160)</f>
+        <f t="shared" si="2"/>
         <v>12705.657285000001</v>
       </c>
       <c r="T160">
         <v>4</v>
       </c>
     </row>
-    <row r="161" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>22</v>
       </c>
@@ -11187,14 +11187,14 @@
         <v>139</v>
       </c>
       <c r="S161" s="4">
-        <f>PRODUCT(Q161,R161)</f>
+        <f t="shared" si="2"/>
         <v>12827.351615849999</v>
       </c>
       <c r="T161">
         <v>3</v>
       </c>
     </row>
-    <row r="162" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>16</v>
       </c>
@@ -11250,14 +11250,14 @@
         <v>182</v>
       </c>
       <c r="S162" s="4">
-        <f>PRODUCT(Q162,R162)</f>
+        <f t="shared" si="2"/>
         <v>12868.592167340001</v>
       </c>
       <c r="T162">
         <v>4</v>
       </c>
     </row>
-    <row r="163" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>22</v>
       </c>
@@ -11313,14 +11313,14 @@
         <v>57</v>
       </c>
       <c r="S163" s="4">
-        <f>PRODUCT(Q163,R163)</f>
+        <f t="shared" si="2"/>
         <v>12891.981463799999</v>
       </c>
       <c r="T163">
         <v>3</v>
       </c>
     </row>
-    <row r="164" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>22</v>
       </c>
@@ -11376,14 +11376,14 @@
         <v>139</v>
       </c>
       <c r="S164" s="4">
-        <f>PRODUCT(Q164,R164)</f>
+        <f t="shared" si="2"/>
         <v>13090.51809602</v>
       </c>
       <c r="T164">
         <v>2</v>
       </c>
     </row>
-    <row r="165" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>23</v>
       </c>
@@ -11439,14 +11439,14 @@
         <v>57</v>
       </c>
       <c r="S165" s="4">
-        <f>PRODUCT(Q165,R165)</f>
+        <f t="shared" si="2"/>
         <v>13146.0243933</v>
       </c>
       <c r="T165">
         <v>3</v>
       </c>
     </row>
-    <row r="166" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>24</v>
       </c>
@@ -11502,14 +11502,14 @@
         <v>139</v>
       </c>
       <c r="S166" s="4">
-        <f>PRODUCT(Q166,R166)</f>
+        <f t="shared" si="2"/>
         <v>13158.96737695</v>
       </c>
       <c r="T166">
         <v>4</v>
       </c>
     </row>
-    <row r="167" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>22</v>
       </c>
@@ -11565,14 +11565,14 @@
         <v>139</v>
       </c>
       <c r="S167" s="4">
-        <f>PRODUCT(Q167,R167)</f>
+        <f t="shared" si="2"/>
         <v>13255.10532583</v>
       </c>
       <c r="T167">
         <v>3</v>
       </c>
     </row>
-    <row r="168" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>23</v>
       </c>
@@ -11628,14 +11628,14 @@
         <v>117</v>
       </c>
       <c r="S168" s="4">
-        <f>PRODUCT(Q168,R168)</f>
+        <f t="shared" si="2"/>
         <v>13265.247726900001</v>
       </c>
       <c r="T168">
         <v>3</v>
       </c>
     </row>
-    <row r="169" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>23</v>
       </c>
@@ -11691,14 +11691,14 @@
         <v>139</v>
       </c>
       <c r="S169" s="4">
-        <f>PRODUCT(Q169,R169)</f>
+        <f t="shared" si="2"/>
         <v>13279.61375857</v>
       </c>
       <c r="T169">
         <v>2</v>
       </c>
     </row>
-    <row r="170" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>23</v>
       </c>
@@ -11754,14 +11754,14 @@
         <v>139</v>
       </c>
       <c r="S170" s="4">
-        <f>PRODUCT(Q170,R170)</f>
+        <f t="shared" si="2"/>
         <v>13339.053643300002</v>
       </c>
       <c r="T170">
         <v>3</v>
       </c>
     </row>
-    <row r="171" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>23</v>
       </c>
@@ -11817,14 +11817,14 @@
         <v>57</v>
       </c>
       <c r="S171" s="4">
-        <f>PRODUCT(Q171,R171)</f>
+        <f t="shared" si="2"/>
         <v>13366.229232899999</v>
       </c>
       <c r="T171">
         <v>2</v>
       </c>
     </row>
-    <row r="172" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>22</v>
       </c>
@@ -11880,14 +11880,14 @@
         <v>57</v>
       </c>
       <c r="S172" s="4">
-        <f>PRODUCT(Q172,R172)</f>
+        <f t="shared" si="2"/>
         <v>13395.300874500001</v>
       </c>
       <c r="T172">
         <v>3</v>
       </c>
     </row>
-    <row r="173" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>24</v>
       </c>
@@ -11943,14 +11943,14 @@
         <v>57</v>
       </c>
       <c r="S173" s="4">
-        <f>PRODUCT(Q173,R173)</f>
+        <f t="shared" si="2"/>
         <v>13441.579174500001</v>
       </c>
       <c r="T173">
         <v>2</v>
       </c>
     </row>
-    <row r="174" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>22</v>
       </c>
@@ -12006,14 +12006,14 @@
         <v>117</v>
       </c>
       <c r="S174" s="4">
-        <f>PRODUCT(Q174,R174)</f>
+        <f t="shared" si="2"/>
         <v>13691.707707600001</v>
       </c>
       <c r="T174">
         <v>2</v>
       </c>
     </row>
-    <row r="175" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>24</v>
       </c>
@@ -12069,14 +12069,14 @@
         <v>57</v>
       </c>
       <c r="S175" s="4">
-        <f>PRODUCT(Q175,R175)</f>
+        <f t="shared" si="2"/>
         <v>13707.0942204</v>
       </c>
       <c r="T175">
         <v>3</v>
       </c>
     </row>
-    <row r="176" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>24</v>
       </c>
@@ -12132,14 +12132,14 @@
         <v>152</v>
       </c>
       <c r="S176" s="4">
-        <f>PRODUCT(Q176,R176)</f>
+        <f t="shared" si="2"/>
         <v>13759.802707119999</v>
       </c>
       <c r="T176">
         <v>2</v>
       </c>
     </row>
-    <row r="177" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>24</v>
       </c>
@@ -12195,14 +12195,14 @@
         <v>139</v>
       </c>
       <c r="S177" s="4">
-        <f>PRODUCT(Q177,R177)</f>
+        <f t="shared" si="2"/>
         <v>13766.3397128</v>
       </c>
       <c r="T177">
         <v>4</v>
       </c>
     </row>
-    <row r="178" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>23</v>
       </c>
@@ -12258,14 +12258,14 @@
         <v>57</v>
       </c>
       <c r="S178" s="4">
-        <f>PRODUCT(Q178,R178)</f>
+        <f t="shared" si="2"/>
         <v>13863.7373739</v>
       </c>
       <c r="T178">
         <v>3</v>
       </c>
     </row>
-    <row r="179" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>24</v>
       </c>
@@ -12321,14 +12321,14 @@
         <v>152</v>
       </c>
       <c r="S179" s="4">
-        <f>PRODUCT(Q179,R179)</f>
+        <f t="shared" si="2"/>
         <v>13873.896000159999</v>
       </c>
       <c r="T179">
         <v>3</v>
       </c>
     </row>
-    <row r="180" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>24</v>
       </c>
@@ -12384,14 +12384,14 @@
         <v>57</v>
       </c>
       <c r="S180" s="4">
-        <f>PRODUCT(Q180,R180)</f>
+        <f t="shared" si="2"/>
         <v>14030.556800099999</v>
       </c>
       <c r="T180">
         <v>2</v>
       </c>
     </row>
-    <row r="181" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>22</v>
       </c>
@@ -12447,14 +12447,14 @@
         <v>117</v>
       </c>
       <c r="S181" s="4">
-        <f>PRODUCT(Q181,R181)</f>
+        <f t="shared" si="2"/>
         <v>14062.7808711</v>
       </c>
       <c r="T181">
         <v>3</v>
       </c>
     </row>
-    <row r="182" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>23</v>
       </c>
@@ -12510,14 +12510,14 @@
         <v>139</v>
       </c>
       <c r="S182" s="4">
-        <f>PRODUCT(Q182,R182)</f>
+        <f t="shared" si="2"/>
         <v>14072.9637743</v>
       </c>
       <c r="T182">
         <v>3</v>
       </c>
     </row>
-    <row r="183" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>22</v>
       </c>
@@ -12573,14 +12573,14 @@
         <v>117</v>
       </c>
       <c r="S183" s="4">
-        <f>PRODUCT(Q183,R183)</f>
+        <f t="shared" si="2"/>
         <v>14102.373858299999</v>
       </c>
       <c r="T183">
         <v>2</v>
       </c>
     </row>
-    <row r="184" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>22</v>
       </c>
@@ -12636,14 +12636,14 @@
         <v>57</v>
       </c>
       <c r="S184" s="4">
-        <f>PRODUCT(Q184,R184)</f>
+        <f t="shared" si="2"/>
         <v>14174.7349827</v>
       </c>
       <c r="T184">
         <v>4</v>
       </c>
     </row>
-    <row r="185" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>22</v>
       </c>
@@ -12699,14 +12699,14 @@
         <v>139</v>
       </c>
       <c r="S185" s="4">
-        <f>PRODUCT(Q185,R185)</f>
+        <f t="shared" si="2"/>
         <v>14277.593708500001</v>
       </c>
       <c r="T185">
         <v>2</v>
       </c>
     </row>
-    <row r="186" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>22</v>
       </c>
@@ -12762,14 +12762,14 @@
         <v>139</v>
       </c>
       <c r="S186" s="4">
-        <f>PRODUCT(Q186,R186)</f>
+        <f t="shared" si="2"/>
         <v>14469.101236499999</v>
       </c>
       <c r="T186">
         <v>3</v>
       </c>
     </row>
-    <row r="187" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>16</v>
       </c>
@@ -12825,14 +12825,14 @@
         <v>224</v>
       </c>
       <c r="S187" s="4">
-        <f>PRODUCT(Q187,R187)</f>
+        <f t="shared" si="2"/>
         <v>14568.876230719998</v>
       </c>
       <c r="T187">
         <v>3</v>
       </c>
     </row>
-    <row r="188" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>23</v>
       </c>
@@ -12888,14 +12888,14 @@
         <v>57</v>
       </c>
       <c r="S188" s="4">
-        <f>PRODUCT(Q188,R188)</f>
+        <f t="shared" si="2"/>
         <v>14574.008634</v>
       </c>
       <c r="T188">
         <v>2</v>
       </c>
     </row>
-    <row r="189" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>23</v>
       </c>
@@ -12951,14 +12951,14 @@
         <v>139</v>
       </c>
       <c r="S189" s="4">
-        <f>PRODUCT(Q189,R189)</f>
+        <f t="shared" si="2"/>
         <v>14658.196892099999</v>
       </c>
       <c r="T189">
         <v>3</v>
       </c>
     </row>
-    <row r="190" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>24</v>
       </c>
@@ -13014,14 +13014,14 @@
         <v>152</v>
       </c>
       <c r="S190" s="4">
-        <f>PRODUCT(Q190,R190)</f>
+        <f t="shared" si="2"/>
         <v>14679.68549552</v>
       </c>
       <c r="T190">
         <v>3</v>
       </c>
     </row>
-    <row r="191" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>22</v>
       </c>
@@ -13077,14 +13077,14 @@
         <v>139</v>
       </c>
       <c r="S191" s="4">
-        <f>PRODUCT(Q191,R191)</f>
+        <f t="shared" si="2"/>
         <v>14705.3473462</v>
       </c>
       <c r="T191">
         <v>2</v>
       </c>
     </row>
-    <row r="192" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>23</v>
       </c>
@@ -13140,14 +13140,14 @@
         <v>57</v>
       </c>
       <c r="S192" s="4">
-        <f>PRODUCT(Q192,R192)</f>
+        <f t="shared" si="2"/>
         <v>14722.554612600001</v>
       </c>
       <c r="T192">
         <v>3</v>
       </c>
     </row>
-    <row r="193" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>16</v>
       </c>
@@ -13203,14 +13203,14 @@
         <v>113</v>
       </c>
       <c r="S193" s="4">
-        <f>PRODUCT(Q193,R193)</f>
+        <f t="shared" si="2"/>
         <v>14759.341546</v>
       </c>
       <c r="T193">
         <v>3</v>
       </c>
     </row>
-    <row r="194" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>23</v>
       </c>
@@ -13266,14 +13266,14 @@
         <v>139</v>
       </c>
       <c r="S194" s="4">
-        <f>PRODUCT(Q194,R194)</f>
+        <f t="shared" ref="S194:S257" si="3">PRODUCT(Q194,R194)</f>
         <v>14789.2957429</v>
       </c>
       <c r="T194">
         <v>2</v>
       </c>
     </row>
-    <row r="195" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>24</v>
       </c>
@@ -13329,14 +13329,14 @@
         <v>57</v>
       </c>
       <c r="S195" s="4">
-        <f>PRODUCT(Q195,R195)</f>
+        <f t="shared" si="3"/>
         <v>14865.7448769</v>
       </c>
       <c r="T195">
         <v>3</v>
       </c>
     </row>
-    <row r="196" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>24</v>
       </c>
@@ -13392,14 +13392,14 @@
         <v>57</v>
       </c>
       <c r="S196" s="4">
-        <f>PRODUCT(Q196,R196)</f>
+        <f t="shared" si="3"/>
         <v>15061.298561699999</v>
       </c>
       <c r="T196">
         <v>4</v>
       </c>
     </row>
-    <row r="197" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>24</v>
       </c>
@@ -13455,14 +13455,14 @@
         <v>152</v>
       </c>
       <c r="S197" s="4">
-        <f>PRODUCT(Q197,R197)</f>
+        <f t="shared" si="3"/>
         <v>15151.210155359999</v>
       </c>
       <c r="T197">
         <v>3</v>
       </c>
     </row>
-    <row r="198" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>22</v>
       </c>
@@ -13518,14 +13518,14 @@
         <v>117</v>
       </c>
       <c r="S198" s="4">
-        <f>PRODUCT(Q198,R198)</f>
+        <f t="shared" si="3"/>
         <v>15244.461343800001</v>
       </c>
       <c r="T198">
         <v>3</v>
       </c>
     </row>
-    <row r="199" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>23</v>
       </c>
@@ -13581,14 +13581,14 @@
         <v>57</v>
       </c>
       <c r="S199" s="4">
-        <f>PRODUCT(Q199,R199)</f>
+        <f t="shared" si="3"/>
         <v>15291.721557599998</v>
       </c>
       <c r="T199">
         <v>2</v>
       </c>
     </row>
-    <row r="200" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>24</v>
       </c>
@@ -13644,14 +13644,14 @@
         <v>152</v>
       </c>
       <c r="S200" s="4">
-        <f>PRODUCT(Q200,R200)</f>
+        <f t="shared" si="3"/>
         <v>15336.962305600002</v>
       </c>
       <c r="T200">
         <v>2</v>
       </c>
     </row>
-    <row r="201" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>24</v>
       </c>
@@ -13707,14 +13707,14 @@
         <v>57</v>
       </c>
       <c r="S201" s="4">
-        <f>PRODUCT(Q201,R201)</f>
+        <f t="shared" si="3"/>
         <v>15454.7225253</v>
       </c>
       <c r="T201">
         <v>3</v>
       </c>
     </row>
-    <row r="202" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>22</v>
       </c>
@@ -13770,14 +13770,14 @@
         <v>57</v>
       </c>
       <c r="S202" s="4">
-        <f>PRODUCT(Q202,R202)</f>
+        <f t="shared" si="3"/>
         <v>15479.435502299999</v>
       </c>
       <c r="T202">
         <v>4</v>
       </c>
     </row>
-    <row r="203" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>23</v>
       </c>
@@ -13833,14 +13833,14 @@
         <v>139</v>
       </c>
       <c r="S203" s="4">
-        <f>PRODUCT(Q203,R203)</f>
+        <f t="shared" si="3"/>
         <v>15523.2057905</v>
       </c>
       <c r="T203">
         <v>2</v>
       </c>
     </row>
-    <row r="204" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>22</v>
       </c>
@@ -13896,14 +13896,14 @@
         <v>117</v>
       </c>
       <c r="S204" s="4">
-        <f>PRODUCT(Q204,R204)</f>
+        <f t="shared" si="3"/>
         <v>15655.1275413</v>
       </c>
       <c r="T204">
         <v>3</v>
       </c>
     </row>
-    <row r="205" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>22</v>
       </c>
@@ -13959,14 +13959,14 @@
         <v>139</v>
       </c>
       <c r="S205" s="4">
-        <f>PRODUCT(Q205,R205)</f>
+        <f t="shared" si="3"/>
         <v>15724.017144500001</v>
       </c>
       <c r="T205">
         <v>3</v>
       </c>
     </row>
-    <row r="206" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>16</v>
       </c>
@@ -14022,14 +14022,14 @@
         <v>182</v>
       </c>
       <c r="S206" s="4">
-        <f>PRODUCT(Q206,R206)</f>
+        <f t="shared" si="3"/>
         <v>15833.448640099999</v>
       </c>
       <c r="T206">
         <v>3</v>
       </c>
     </row>
-    <row r="207" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>22</v>
       </c>
@@ -14085,14 +14085,14 @@
         <v>139</v>
       </c>
       <c r="S207" s="4">
-        <f>PRODUCT(Q207,R207)</f>
+        <f t="shared" si="3"/>
         <v>15845.563456600001</v>
       </c>
       <c r="T207">
         <v>4</v>
       </c>
     </row>
-    <row r="208" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>16</v>
       </c>
@@ -14148,14 +14148,14 @@
         <v>224</v>
       </c>
       <c r="S208" s="4">
-        <f>PRODUCT(Q208,R208)</f>
+        <f t="shared" si="3"/>
         <v>15877.339640959999</v>
       </c>
       <c r="T208">
         <v>3</v>
       </c>
     </row>
-    <row r="209" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>16</v>
       </c>
@@ -14211,14 +14211,14 @@
         <v>113</v>
       </c>
       <c r="S209" s="4">
-        <f>PRODUCT(Q209,R209)</f>
+        <f t="shared" si="3"/>
         <v>15943.328810200002</v>
       </c>
       <c r="T209">
         <v>2</v>
       </c>
     </row>
-    <row r="210" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>16</v>
       </c>
@@ -14274,14 +14274,14 @@
         <v>224</v>
       </c>
       <c r="S210" s="4">
-        <f>PRODUCT(Q210,R210)</f>
+        <f t="shared" si="3"/>
         <v>15988.14056448</v>
       </c>
       <c r="T210">
         <v>2</v>
       </c>
     </row>
-    <row r="211" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>23</v>
       </c>
@@ -14337,14 +14337,14 @@
         <v>57</v>
       </c>
       <c r="S211" s="4">
-        <f>PRODUCT(Q211,R211)</f>
+        <f t="shared" si="3"/>
         <v>15998.174336400001</v>
       </c>
       <c r="T211">
         <v>3</v>
       </c>
     </row>
-    <row r="212" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>23</v>
       </c>
@@ -14400,14 +14400,14 @@
         <v>139</v>
       </c>
       <c r="S212" s="4">
-        <f>PRODUCT(Q212,R212)</f>
+        <f t="shared" si="3"/>
         <v>16034.659126100001</v>
       </c>
       <c r="T212">
         <v>4</v>
       </c>
     </row>
-    <row r="213" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>22</v>
       </c>
@@ -14463,14 +14463,14 @@
         <v>57</v>
       </c>
       <c r="S213" s="4">
-        <f>PRODUCT(Q213,R213)</f>
+        <f t="shared" si="3"/>
         <v>16087.642459799999</v>
       </c>
       <c r="T213">
         <v>4</v>
       </c>
     </row>
-    <row r="214" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>24</v>
       </c>
@@ -14526,14 +14526,14 @@
         <v>152</v>
       </c>
       <c r="S214" s="4">
-        <f>PRODUCT(Q214,R214)</f>
+        <f t="shared" si="3"/>
         <v>16142.751727999999</v>
       </c>
       <c r="T214">
         <v>2</v>
       </c>
     </row>
-    <row r="215" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>22</v>
       </c>
@@ -14589,14 +14589,14 @@
         <v>139</v>
       </c>
       <c r="S215" s="4">
-        <f>PRODUCT(Q215,R215)</f>
+        <f t="shared" si="3"/>
         <v>16151.770768299999</v>
       </c>
       <c r="T215">
         <v>3</v>
       </c>
     </row>
-    <row r="216" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>23</v>
       </c>
@@ -14652,14 +14652,14 @@
         <v>139</v>
       </c>
       <c r="S216" s="4">
-        <f>PRODUCT(Q216,R216)</f>
+        <f t="shared" si="3"/>
         <v>16235.719165</v>
       </c>
       <c r="T216">
         <v>3</v>
       </c>
     </row>
-    <row r="217" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>24</v>
       </c>
@@ -14715,14 +14715,14 @@
         <v>57</v>
       </c>
       <c r="S217" s="4">
-        <f>PRODUCT(Q217,R217)</f>
+        <f t="shared" si="3"/>
         <v>16287.6938037</v>
       </c>
       <c r="T217">
         <v>4</v>
       </c>
     </row>
-    <row r="218" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>22</v>
       </c>
@@ -14778,14 +14778,14 @@
         <v>117</v>
       </c>
       <c r="S218" s="4">
-        <f>PRODUCT(Q218,R218)</f>
+        <f t="shared" si="3"/>
         <v>16483.468189499999</v>
       </c>
       <c r="T218">
         <v>4</v>
       </c>
     </row>
-    <row r="219" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>24</v>
       </c>
@@ -14841,14 +14841,14 @@
         <v>152</v>
       </c>
       <c r="S219" s="4">
-        <f>PRODUCT(Q219,R219)</f>
+        <f t="shared" si="3"/>
         <v>16540.496496799999</v>
       </c>
       <c r="T219">
         <v>4</v>
       </c>
     </row>
-    <row r="220" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>16</v>
       </c>
@@ -14904,14 +14904,14 @@
         <v>224</v>
       </c>
       <c r="S220" s="4">
-        <f>PRODUCT(Q220,R220)</f>
+        <f t="shared" si="3"/>
         <v>16617.354797119999</v>
       </c>
       <c r="T220">
         <v>3</v>
       </c>
     </row>
-    <row r="221" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>16</v>
       </c>
@@ -14967,14 +14967,14 @@
         <v>113</v>
       </c>
       <c r="S221" s="4">
-        <f>PRODUCT(Q221,R221)</f>
+        <f t="shared" si="3"/>
         <v>16697.326112700001</v>
       </c>
       <c r="T221">
         <v>3</v>
       </c>
     </row>
-    <row r="222" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>23</v>
       </c>
@@ -15030,14 +15030,14 @@
         <v>57</v>
       </c>
       <c r="S222" s="4">
-        <f>PRODUCT(Q222,R222)</f>
+        <f t="shared" si="3"/>
         <v>16715.887282799999</v>
       </c>
       <c r="T222">
         <v>3</v>
       </c>
     </row>
-    <row r="223" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>24</v>
       </c>
@@ -15093,14 +15093,14 @@
         <v>152</v>
       </c>
       <c r="S223" s="4">
-        <f>PRODUCT(Q223,R223)</f>
+        <f t="shared" si="3"/>
         <v>16796.2100488</v>
       </c>
       <c r="T223">
         <v>3</v>
       </c>
     </row>
-    <row r="224" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>24</v>
       </c>
@@ -15156,14 +15156,14 @@
         <v>57</v>
       </c>
       <c r="S224" s="4">
-        <f>PRODUCT(Q224,R224)</f>
+        <f t="shared" si="3"/>
         <v>16876.671435</v>
       </c>
       <c r="T224">
         <v>4</v>
       </c>
     </row>
-    <row r="225" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>23</v>
       </c>
@@ -15219,14 +15219,14 @@
         <v>139</v>
       </c>
       <c r="S225" s="4">
-        <f>PRODUCT(Q225,R225)</f>
+        <f t="shared" si="3"/>
         <v>16969.629226500001</v>
       </c>
       <c r="T225">
         <v>3</v>
       </c>
     </row>
-    <row r="226" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>23</v>
       </c>
@@ -15282,14 +15282,14 @@
         <v>57</v>
       </c>
       <c r="S226" s="4">
-        <f>PRODUCT(Q226,R226)</f>
+        <f t="shared" si="3"/>
         <v>17103.325773299999</v>
       </c>
       <c r="T226">
         <v>4</v>
       </c>
     </row>
-    <row r="227" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>16</v>
       </c>
@@ -15345,14 +15345,14 @@
         <v>113</v>
       </c>
       <c r="S227" s="4">
-        <f>PRODUCT(Q227,R227)</f>
+        <f t="shared" si="3"/>
         <v>17124.5762086</v>
       </c>
       <c r="T227">
         <v>3</v>
       </c>
     </row>
-    <row r="228" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>22</v>
       </c>
@@ -15408,14 +15408,14 @@
         <v>139</v>
       </c>
       <c r="S228" s="4">
-        <f>PRODUCT(Q228,R228)</f>
+        <f t="shared" si="3"/>
         <v>17168.223961399999</v>
       </c>
       <c r="T228">
         <v>4</v>
       </c>
     </row>
-    <row r="229" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>16</v>
       </c>
@@ -15471,14 +15471,14 @@
         <v>182</v>
       </c>
       <c r="S229" s="4">
-        <f>PRODUCT(Q229,R229)</f>
+        <f t="shared" si="3"/>
         <v>17269.823409019999</v>
       </c>
       <c r="T229">
         <v>2</v>
       </c>
     </row>
-    <row r="230" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>16</v>
       </c>
@@ -15534,14 +15534,14 @@
         <v>224</v>
       </c>
       <c r="S230" s="4">
-        <f>PRODUCT(Q230,R230)</f>
+        <f t="shared" si="3"/>
         <v>17364.609149439999</v>
       </c>
       <c r="T230">
         <v>2</v>
       </c>
     </row>
-    <row r="231" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>16</v>
       </c>
@@ -15597,14 +15597,14 @@
         <v>224</v>
       </c>
       <c r="S231" s="4">
-        <f>PRODUCT(Q231,R231)</f>
+        <f t="shared" si="3"/>
         <v>17403.749762560001</v>
       </c>
       <c r="T231">
         <v>3</v>
       </c>
     </row>
-    <row r="232" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>16</v>
       </c>
@@ -15660,14 +15660,14 @@
         <v>182</v>
       </c>
       <c r="S232" s="4">
-        <f>PRODUCT(Q232,R232)</f>
+        <f t="shared" si="3"/>
         <v>17492.9764282</v>
       </c>
       <c r="T232">
         <v>3</v>
       </c>
     </row>
-    <row r="233" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>22</v>
       </c>
@@ -15723,14 +15723,14 @@
         <v>139</v>
       </c>
       <c r="S233" s="4">
-        <f>PRODUCT(Q233,R233)</f>
+        <f t="shared" si="3"/>
         <v>17595.977599099999</v>
       </c>
       <c r="T233">
         <v>4</v>
       </c>
     </row>
-    <row r="234" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>24</v>
       </c>
@@ -15786,14 +15786,14 @@
         <v>152</v>
       </c>
       <c r="S234" s="4">
-        <f>PRODUCT(Q234,R234)</f>
+        <f t="shared" si="3"/>
         <v>17601.999456000001</v>
       </c>
       <c r="T234">
         <v>3</v>
       </c>
     </row>
-    <row r="235" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>23</v>
       </c>
@@ -15849,14 +15849,14 @@
         <v>139</v>
       </c>
       <c r="S235" s="4">
-        <f>PRODUCT(Q235,R235)</f>
+        <f t="shared" si="3"/>
         <v>17679.9259819</v>
       </c>
       <c r="T235">
         <v>4</v>
       </c>
     </row>
-    <row r="236" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>24</v>
       </c>
@@ -15912,14 +15912,14 @@
         <v>139</v>
       </c>
       <c r="S236" s="4">
-        <f>PRODUCT(Q236,R236)</f>
+        <f t="shared" si="3"/>
         <v>17698.232476500001</v>
       </c>
       <c r="T236">
         <v>3</v>
       </c>
     </row>
-    <row r="237" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>22</v>
       </c>
@@ -15975,14 +15975,14 @@
         <v>117</v>
       </c>
       <c r="S237" s="4">
-        <f>PRODUCT(Q237,R237)</f>
+        <f t="shared" si="3"/>
         <v>17881.346398499998</v>
       </c>
       <c r="T237">
         <v>4</v>
       </c>
     </row>
-    <row r="238" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>16</v>
       </c>
@@ -16038,14 +16038,14 @@
         <v>113</v>
       </c>
       <c r="S238" s="4">
-        <f>PRODUCT(Q238,R238)</f>
+        <f t="shared" si="3"/>
         <v>17939.954715599997</v>
       </c>
       <c r="T238">
         <v>2</v>
       </c>
     </row>
-    <row r="239" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>16</v>
       </c>
@@ -16101,14 +16101,14 @@
         <v>224</v>
       </c>
       <c r="S239" s="4">
-        <f>PRODUCT(Q239,R239)</f>
+        <f t="shared" si="3"/>
         <v>18104.624350400001</v>
       </c>
       <c r="T239">
         <v>2</v>
       </c>
     </row>
-    <row r="240" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>16</v>
       </c>
@@ -16164,14 +16164,14 @@
         <v>113</v>
       </c>
       <c r="S240" s="4">
-        <f>PRODUCT(Q240,R240)</f>
+        <f t="shared" si="3"/>
         <v>18224.882983900003</v>
       </c>
       <c r="T240">
         <v>3</v>
       </c>
     </row>
-    <row r="241" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>24</v>
       </c>
@@ -16227,14 +16227,14 @@
         <v>152</v>
       </c>
       <c r="S241" s="4">
-        <f>PRODUCT(Q241,R241)</f>
+        <f t="shared" si="3"/>
         <v>18253.240978399997</v>
       </c>
       <c r="T241">
         <v>4</v>
       </c>
     </row>
-    <row r="242" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>16</v>
       </c>
@@ -16290,14 +16290,14 @@
         <v>113</v>
       </c>
       <c r="S242" s="4">
-        <f>PRODUCT(Q242,R242)</f>
+        <f t="shared" si="3"/>
         <v>18304.232804300002</v>
       </c>
       <c r="T242">
         <v>4</v>
       </c>
     </row>
-    <row r="243" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>22</v>
       </c>
@@ -16353,14 +16353,14 @@
         <v>117</v>
       </c>
       <c r="S243" s="4">
-        <f>PRODUCT(Q243,R243)</f>
+        <f t="shared" si="3"/>
         <v>18403.767369000001</v>
       </c>
       <c r="T243">
         <v>4</v>
       </c>
     </row>
-    <row r="244" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>23</v>
       </c>
@@ -16416,14 +16416,14 @@
         <v>139</v>
       </c>
       <c r="S244" s="4">
-        <f>PRODUCT(Q244,R244)</f>
+        <f t="shared" si="3"/>
         <v>18413.836057299999</v>
       </c>
       <c r="T244">
         <v>4</v>
       </c>
     </row>
-    <row r="245" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>16</v>
       </c>
@@ -16479,14 +16479,14 @@
         <v>182</v>
       </c>
       <c r="S245" s="4">
-        <f>PRODUCT(Q245,R245)</f>
+        <f t="shared" si="3"/>
         <v>18436.9824548</v>
       </c>
       <c r="T245">
         <v>3</v>
       </c>
     </row>
-    <row r="246" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>23</v>
       </c>
@@ -16542,14 +16542,14 @@
         <v>57</v>
       </c>
       <c r="S246" s="4">
-        <f>PRODUCT(Q246,R246)</f>
+        <f t="shared" si="3"/>
         <v>18619.067772599999</v>
       </c>
       <c r="T246">
         <v>4</v>
       </c>
     </row>
-    <row r="247" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>16</v>
       </c>
@@ -16605,14 +16605,14 @@
         <v>182</v>
       </c>
       <c r="S247" s="4">
-        <f>PRODUCT(Q247,R247)</f>
+        <f t="shared" si="3"/>
         <v>18700.7161796</v>
       </c>
       <c r="T247">
         <v>3</v>
       </c>
     </row>
-    <row r="248" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>16</v>
       </c>
@@ -16668,14 +16668,14 @@
         <v>224</v>
       </c>
       <c r="S248" s="4">
-        <f>PRODUCT(Q248,R248)</f>
+        <f t="shared" si="3"/>
         <v>18817.23906272</v>
       </c>
       <c r="T248">
         <v>4</v>
       </c>
     </row>
-    <row r="249" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>16</v>
       </c>
@@ -16731,14 +16731,14 @@
         <v>224</v>
       </c>
       <c r="S249" s="4">
-        <f>PRODUCT(Q249,R249)</f>
+        <f t="shared" si="3"/>
         <v>18848.05860896</v>
       </c>
       <c r="T249">
         <v>3</v>
       </c>
     </row>
-    <row r="250" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>16</v>
       </c>
@@ -16794,14 +16794,14 @@
         <v>182</v>
       </c>
       <c r="S250" s="4">
-        <f>PRODUCT(Q250,R250)</f>
+        <f t="shared" si="3"/>
         <v>18998.0249186</v>
       </c>
       <c r="T250">
         <v>2</v>
       </c>
     </row>
-    <row r="251" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>24</v>
       </c>
@@ -16857,14 +16857,14 @@
         <v>139</v>
       </c>
       <c r="S251" s="4">
-        <f>PRODUCT(Q251,R251)</f>
+        <f t="shared" si="3"/>
         <v>19080.469409900001</v>
       </c>
       <c r="T251">
         <v>2</v>
       </c>
     </row>
-    <row r="252" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>24</v>
       </c>
@@ -16920,14 +16920,14 @@
         <v>152</v>
       </c>
       <c r="S252" s="4">
-        <f>PRODUCT(Q252,R252)</f>
+        <f t="shared" si="3"/>
         <v>19113.877427200001</v>
       </c>
       <c r="T252">
         <v>4</v>
       </c>
     </row>
-    <row r="253" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>23</v>
       </c>
@@ -16983,14 +16983,14 @@
         <v>117</v>
       </c>
       <c r="S253" s="4">
-        <f>PRODUCT(Q253,R253)</f>
+        <f t="shared" si="3"/>
         <v>19124.3335257</v>
       </c>
       <c r="T253">
         <v>3</v>
       </c>
     </row>
-    <row r="254" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>16</v>
       </c>
@@ -17046,14 +17046,14 @@
         <v>113</v>
       </c>
       <c r="S254" s="4">
-        <f>PRODUCT(Q254,R254)</f>
+        <f t="shared" si="3"/>
         <v>19179.7198646</v>
       </c>
       <c r="T254">
         <v>3</v>
       </c>
     </row>
-    <row r="255" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
         <v>16</v>
       </c>
@@ -17109,14 +17109,14 @@
         <v>113</v>
       </c>
       <c r="S255" s="4">
-        <f>PRODUCT(Q255,R255)</f>
+        <f t="shared" si="3"/>
         <v>19467.511586799999</v>
       </c>
       <c r="T255">
         <v>2</v>
       </c>
     </row>
-    <row r="256" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
         <v>23</v>
       </c>
@@ -17172,14 +17172,14 @@
         <v>57</v>
       </c>
       <c r="S256" s="4">
-        <f>PRODUCT(Q256,R256)</f>
+        <f t="shared" si="3"/>
         <v>19526.275024500002</v>
       </c>
       <c r="T256">
         <v>4</v>
       </c>
     </row>
-    <row r="257" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
         <v>16</v>
       </c>
@@ -17235,14 +17235,14 @@
         <v>224</v>
       </c>
       <c r="S257" s="4">
-        <f>PRODUCT(Q257,R257)</f>
+        <f t="shared" si="3"/>
         <v>19588.073816640001</v>
       </c>
       <c r="T257">
         <v>3</v>
       </c>
     </row>
-    <row r="258" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
         <v>16</v>
       </c>
@@ -17298,14 +17298,14 @@
         <v>182</v>
       </c>
       <c r="S258" s="4">
-        <f>PRODUCT(Q258,R258)</f>
+        <f t="shared" ref="S258:S321" si="4">PRODUCT(Q258,R258)</f>
         <v>19942.030981600001</v>
       </c>
       <c r="T258">
         <v>2</v>
       </c>
     </row>
-    <row r="259" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
         <v>16</v>
       </c>
@@ -17361,14 +17361,14 @@
         <v>182</v>
       </c>
       <c r="S259" s="4">
-        <f>PRODUCT(Q259,R259)</f>
+        <f t="shared" si="4"/>
         <v>20128.427482800002</v>
       </c>
       <c r="T259">
         <v>4</v>
       </c>
     </row>
-    <row r="260" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
         <v>24</v>
       </c>
@@ -17424,14 +17424,14 @@
         <v>139</v>
       </c>
       <c r="S260" s="4">
-        <f>PRODUCT(Q260,R260)</f>
+        <f t="shared" si="4"/>
         <v>20291.8291814</v>
       </c>
       <c r="T260">
         <v>3</v>
       </c>
     </row>
-    <row r="261" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
         <v>16</v>
       </c>
@@ -17487,14 +17487,14 @@
         <v>224</v>
       </c>
       <c r="S261" s="4">
-        <f>PRODUCT(Q261,R261)</f>
+        <f t="shared" si="4"/>
         <v>20329.292511359999</v>
       </c>
       <c r="T261">
         <v>4</v>
       </c>
     </row>
-    <row r="262" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
         <v>16</v>
       </c>
@@ -17550,14 +17550,14 @@
         <v>113</v>
       </c>
       <c r="S262" s="4">
-        <f>PRODUCT(Q262,R262)</f>
+        <f t="shared" si="4"/>
         <v>20417.822388099998</v>
       </c>
       <c r="T262">
         <v>4</v>
       </c>
     </row>
-    <row r="263" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
         <v>24</v>
       </c>
@@ -17613,14 +17613,14 @@
         <v>139</v>
       </c>
       <c r="S263" s="4">
-        <f>PRODUCT(Q263,R263)</f>
+        <f t="shared" si="4"/>
         <v>20459.052547599997</v>
       </c>
       <c r="T263">
         <v>3</v>
       </c>
     </row>
-    <row r="264" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
         <v>16</v>
       </c>
@@ -17676,14 +17676,14 @@
         <v>182</v>
       </c>
       <c r="S264" s="4">
-        <f>PRODUCT(Q264,R264)</f>
+        <f t="shared" si="4"/>
         <v>20497.344048999999</v>
       </c>
       <c r="T264">
         <v>3</v>
       </c>
     </row>
-    <row r="265" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
         <v>23</v>
       </c>
@@ -17739,14 +17739,14 @@
         <v>117</v>
       </c>
       <c r="S265" s="4">
-        <f>PRODUCT(Q265,R265)</f>
+        <f t="shared" si="4"/>
         <v>20551.202614799997</v>
       </c>
       <c r="T265">
         <v>2</v>
       </c>
     </row>
-    <row r="266" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
         <v>16</v>
       </c>
@@ -17802,14 +17802,14 @@
         <v>113</v>
       </c>
       <c r="S266" s="4">
-        <f>PRODUCT(Q266,R266)</f>
+        <f t="shared" si="4"/>
         <v>20707.276769700002</v>
       </c>
       <c r="T266">
         <v>3</v>
       </c>
     </row>
-    <row r="267" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
         <v>16</v>
       </c>
@@ -17865,14 +17865,14 @@
         <v>224</v>
       </c>
       <c r="S267" s="4">
-        <f>PRODUCT(Q267,R267)</f>
+        <f t="shared" si="4"/>
         <v>21069.307750399999</v>
       </c>
       <c r="T267">
         <v>4</v>
       </c>
     </row>
-    <row r="268" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
         <v>16</v>
       </c>
@@ -17928,14 +17928,14 @@
         <v>182</v>
       </c>
       <c r="S268" s="4">
-        <f>PRODUCT(Q268,R268)</f>
+        <f t="shared" si="4"/>
         <v>21441.350112</v>
       </c>
       <c r="T268">
         <v>3</v>
       </c>
     </row>
-    <row r="269" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
         <v>24</v>
       </c>
@@ -17991,14 +17991,14 @@
         <v>139</v>
       </c>
       <c r="S269" s="4">
-        <f>PRODUCT(Q269,R269)</f>
+        <f t="shared" si="4"/>
         <v>21742.071281</v>
       </c>
       <c r="T269">
         <v>2</v>
       </c>
     </row>
-    <row r="270" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
         <v>23</v>
       </c>
@@ -18054,14 +18054,14 @@
         <v>117</v>
       </c>
       <c r="S270" s="4">
-        <f>PRODUCT(Q270,R270)</f>
+        <f t="shared" si="4"/>
         <v>21815.347834799999</v>
       </c>
       <c r="T270">
         <v>3</v>
       </c>
     </row>
-    <row r="271" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
         <v>24</v>
       </c>
@@ -18117,14 +18117,14 @@
         <v>139</v>
       </c>
       <c r="S271" s="4">
-        <f>PRODUCT(Q271,R271)</f>
+        <f t="shared" si="4"/>
         <v>21835.514767700002</v>
       </c>
       <c r="T271">
         <v>4</v>
       </c>
     </row>
-    <row r="272" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
         <v>16</v>
       </c>
@@ -18180,14 +18180,14 @@
         <v>113</v>
       </c>
       <c r="S272" s="4">
-        <f>PRODUCT(Q272,R272)</f>
+        <f t="shared" si="4"/>
         <v>21945.3792932</v>
       </c>
       <c r="T272">
         <v>4</v>
       </c>
     </row>
-    <row r="273" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
         <v>23</v>
       </c>
@@ -18243,14 +18243,14 @@
         <v>117</v>
       </c>
       <c r="S273" s="4">
-        <f>PRODUCT(Q273,R273)</f>
+        <f t="shared" si="4"/>
         <v>21974.418039600001</v>
       </c>
       <c r="T273">
         <v>3</v>
       </c>
     </row>
-    <row r="274" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
         <v>16</v>
       </c>
@@ -18306,14 +18306,14 @@
         <v>182</v>
       </c>
       <c r="S274" s="4">
-        <f>PRODUCT(Q274,R274)</f>
+        <f t="shared" si="4"/>
         <v>21993.3381668</v>
       </c>
       <c r="T274">
         <v>4</v>
       </c>
     </row>
-    <row r="275" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
         <v>24</v>
       </c>
@@ -18369,14 +18369,14 @@
         <v>139</v>
       </c>
       <c r="S275" s="4">
-        <f>PRODUCT(Q275,R275)</f>
+        <f t="shared" si="4"/>
         <v>22064.7016234</v>
       </c>
       <c r="T275">
         <v>3</v>
       </c>
     </row>
-    <row r="276" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
         <v>16</v>
       </c>
@@ -18432,14 +18432,14 @@
         <v>182</v>
       </c>
       <c r="S276" s="4">
-        <f>PRODUCT(Q276,R276)</f>
+        <f t="shared" si="4"/>
         <v>22937.3441752</v>
       </c>
       <c r="T276">
         <v>4</v>
       </c>
     </row>
-    <row r="277" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
         <v>24</v>
       </c>
@@ -18495,14 +18495,14 @@
         <v>139</v>
       </c>
       <c r="S277" s="4">
-        <f>PRODUCT(Q277,R277)</f>
+        <f t="shared" si="4"/>
         <v>23188.494703100001</v>
       </c>
       <c r="T277">
         <v>3</v>
       </c>
     </row>
-    <row r="278" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
         <v>23</v>
       </c>
@@ -18558,14 +18558,14 @@
         <v>117</v>
       </c>
       <c r="S278" s="4">
-        <f>PRODUCT(Q278,R278)</f>
+        <f t="shared" si="4"/>
         <v>23310.222074100002</v>
       </c>
       <c r="T278">
         <v>2</v>
       </c>
     </row>
-    <row r="279" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
         <v>24</v>
       </c>
@@ -18621,14 +18621,14 @@
         <v>139</v>
       </c>
       <c r="S279" s="4">
-        <f>PRODUCT(Q279,R279)</f>
+        <f t="shared" si="4"/>
         <v>23514.943639600002</v>
       </c>
       <c r="T279">
         <v>2</v>
       </c>
     </row>
-    <row r="280" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
         <v>23</v>
       </c>
@@ -18684,14 +18684,14 @@
         <v>117</v>
       </c>
       <c r="S280" s="4">
-        <f>PRODUCT(Q280,R280)</f>
+        <f t="shared" si="4"/>
         <v>23769.480500999998</v>
       </c>
       <c r="T280">
         <v>3</v>
       </c>
     </row>
-    <row r="281" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
         <v>24</v>
       </c>
@@ -18747,14 +18747,14 @@
         <v>139</v>
       </c>
       <c r="S281" s="4">
-        <f>PRODUCT(Q281,R281)</f>
+        <f t="shared" si="4"/>
         <v>24632.701520000002</v>
       </c>
       <c r="T281">
         <v>4</v>
       </c>
     </row>
-    <row r="282" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
         <v>23</v>
       </c>
@@ -18810,14 +18810,14 @@
         <v>117</v>
       </c>
       <c r="S282" s="4">
-        <f>PRODUCT(Q282,R282)</f>
+        <f t="shared" si="4"/>
         <v>24801.277819499999</v>
       </c>
       <c r="T282">
         <v>3</v>
       </c>
     </row>
-    <row r="283" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
         <v>23</v>
       </c>
@@ -18873,14 +18873,14 @@
         <v>117</v>
       </c>
       <c r="S283" s="4">
-        <f>PRODUCT(Q283,R283)</f>
+        <f t="shared" si="4"/>
         <v>24955.631836199998</v>
       </c>
       <c r="T283">
         <v>4</v>
       </c>
     </row>
-    <row r="284" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
         <v>24</v>
       </c>
@@ -18936,14 +18936,14 @@
         <v>139</v>
       </c>
       <c r="S284" s="4">
-        <f>PRODUCT(Q284,R284)</f>
+        <f t="shared" si="4"/>
         <v>24961.367061700003</v>
       </c>
       <c r="T284">
         <v>3</v>
       </c>
     </row>
-    <row r="285" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
         <v>23</v>
       </c>
@@ -18999,14 +18999,14 @@
         <v>117</v>
       </c>
       <c r="S285" s="4">
-        <f>PRODUCT(Q285,R285)</f>
+        <f t="shared" si="4"/>
         <v>25264.354740300001</v>
       </c>
       <c r="T285">
         <v>2</v>
       </c>
     </row>
-    <row r="286" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
         <v>24</v>
       </c>
@@ -19062,14 +19062,14 @@
         <v>139</v>
       </c>
       <c r="S286" s="4">
-        <f>PRODUCT(Q286,R286)</f>
+        <f t="shared" si="4"/>
         <v>26459.9378211</v>
       </c>
       <c r="T286">
         <v>4</v>
       </c>
     </row>
-    <row r="287" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
         <v>23</v>
       </c>
@@ -19125,14 +19125,14 @@
         <v>117</v>
       </c>
       <c r="S287" s="4">
-        <f>PRODUCT(Q287,R287)</f>
+        <f t="shared" si="4"/>
         <v>26755.410532499998</v>
       </c>
       <c r="T287">
         <v>3</v>
       </c>
     </row>
-    <row r="288" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
         <v>23</v>
       </c>
@@ -19188,14 +19188,14 @@
         <v>117</v>
       </c>
       <c r="S288" s="4">
-        <f>PRODUCT(Q288,R288)</f>
+        <f t="shared" si="4"/>
         <v>28172.587470300001</v>
       </c>
       <c r="T288">
         <v>4</v>
       </c>
     </row>
-    <row r="289" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
         <v>23</v>
       </c>
@@ -19251,7 +19251,7 @@
         <v>117</v>
       </c>
       <c r="S289" s="4">
-        <f>PRODUCT(Q289,R289)</f>
+        <f t="shared" si="4"/>
         <v>30431.173675500002</v>
       </c>
       <c r="T289">
@@ -19259,11 +19259,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:T289" xr:uid="{5D0BB158-B6F1-40DE-B943-200B2E46B926}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:T289">
-      <sortCondition ref="S1:S289"/>
-    </sortState>
-  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:T289">
     <sortCondition ref="A1"/>
   </sortState>

</xml_diff>